<commit_message>
Added detailed data for HRS expt
</commit_message>
<xml_diff>
--- a/Prototypes/Barley/Observed.xlsx
+++ b/Prototypes/Barley/Observed.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18326"/>
   <workbookPr filterPrivacy="1" hidePivotFieldList="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
@@ -10,10 +10,11 @@
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
     <sheet name="MCVPDateEstimates" sheetId="3" r:id="rId2"/>
     <sheet name="Observed" sheetId="1" r:id="rId3"/>
+    <sheet name="HRSData" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="171027"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId4"/>
+    <pivotCache cacheId="10" r:id="rId5"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2344" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2461" uniqueCount="122">
   <si>
     <t>TOS</t>
   </si>
@@ -328,6 +329,69 @@
   <si>
     <t>Barley.Structure.HaunStage.Value()</t>
   </si>
+  <si>
+    <t>Treatment</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Average of PhenologyStage</t>
+  </si>
+  <si>
+    <t>Average of Popn</t>
+  </si>
+  <si>
+    <t>Average of Biomass</t>
+  </si>
+  <si>
+    <t>Average of LAI</t>
+  </si>
+  <si>
+    <t>Average of Height</t>
+  </si>
+  <si>
+    <t>Average of HeadWt</t>
+  </si>
+  <si>
+    <t>Average of HeadPSM</t>
+  </si>
+  <si>
+    <t>Average of Gleaf</t>
+  </si>
+  <si>
+    <t>Average of Dleaf</t>
+  </si>
+  <si>
+    <t>Average of GY</t>
+  </si>
+  <si>
+    <t>Average of 100SeedWt</t>
+  </si>
+  <si>
+    <t>DD</t>
+  </si>
+  <si>
+    <t>DI</t>
+  </si>
+  <si>
+    <t>II</t>
+  </si>
+  <si>
+    <t>StemWt</t>
+  </si>
+  <si>
+    <t>Barley_HRSRO-DD_1</t>
+  </si>
+  <si>
+    <t>Barley_HRSRO-DI_1</t>
+  </si>
+  <si>
+    <t>Barley_HRSRO-II_1</t>
+  </si>
+  <si>
+    <t>Grimmett</t>
+  </si>
 </sst>
 </file>
 
@@ -350,15 +414,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -381,11 +451,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -414,6 +493,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -10132,7 +10216,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{BBEC5F0E-CDED-45B0-8AC4-7B30D923FEED}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" compact="0" compactData="0" gridDropZones="1" multipleFieldFilters="0" chartFormat="2">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{BBEC5F0E-CDED-45B0-8AC4-7B30D923FEED}" name="PivotTable1" cacheId="10" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" compact="0" compactData="0" gridDropZones="1" multipleFieldFilters="0" chartFormat="2">
   <location ref="A4:J24" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="2" colPageCount="1"/>
   <pivotFields count="9">
     <pivotField compact="0" outline="0" subtotalTop="0" showAll="0"/>
@@ -12580,10 +12664,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O718"/>
+  <dimension ref="A1:W762"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" topLeftCell="D709" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L719" sqref="L719:W762"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -12598,7 +12682,7 @@
     <col min="11" max="11" width="10.15625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="3" t="s">
         <v>13</v>
       </c>
@@ -12632,8 +12716,44 @@
       <c r="K1" s="4" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="L1" t="s">
+        <v>103</v>
+      </c>
+      <c r="M1" t="s">
+        <v>104</v>
+      </c>
+      <c r="N1" t="s">
+        <v>117</v>
+      </c>
+      <c r="O1" t="s">
+        <v>105</v>
+      </c>
+      <c r="P1" t="s">
+        <v>106</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>107</v>
+      </c>
+      <c r="R1" t="s">
+        <v>108</v>
+      </c>
+      <c r="S1" t="s">
+        <v>109</v>
+      </c>
+      <c r="T1" t="s">
+        <v>110</v>
+      </c>
+      <c r="U1" t="s">
+        <v>111</v>
+      </c>
+      <c r="V1" t="s">
+        <v>112</v>
+      </c>
+      <c r="W1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="3" t="str">
         <f>"MCVP"&amp;F2&amp;"Cv"&amp;C2&amp;"TOS"&amp;D2</f>
         <v>MCVPBirchipCvBaudinTOS13-may</v>
@@ -12666,7 +12786,7 @@
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="3" t="str">
         <f t="shared" ref="A3:A66" si="0">"MCVP"&amp;F3&amp;"Cv"&amp;C3&amp;"TOS"&amp;D3</f>
         <v>MCVPBirchipCvBulokeTOS13-may</v>
@@ -12699,7 +12819,7 @@
       <c r="N3" s="1"/>
       <c r="O3" s="1"/>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="3" t="str">
         <f t="shared" si="0"/>
         <v>MCVPBirchipCvCapstanTOS13-may</v>
@@ -12732,7 +12852,7 @@
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="3" t="str">
         <f t="shared" si="0"/>
         <v>MCVPBirchipCvCommanderTOS13-may</v>
@@ -12765,7 +12885,7 @@
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="3" t="str">
         <f t="shared" si="0"/>
         <v>MCVPBirchipCvFleetTOS13-may</v>
@@ -12798,7 +12918,7 @@
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="3" t="str">
         <f t="shared" si="0"/>
         <v>MCVPBirchipCvHindmarshTOS13-may</v>
@@ -12831,7 +12951,7 @@
       <c r="N7" s="1"/>
       <c r="O7" s="1"/>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="3" t="str">
         <f t="shared" si="0"/>
         <v>MCVPBirchipCvKeelTOS13-may</v>
@@ -12864,7 +12984,7 @@
       <c r="N8" s="1"/>
       <c r="O8" s="1"/>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="3" t="str">
         <f t="shared" si="0"/>
         <v>MCVPBirchipCvOxfordTOS13-may</v>
@@ -12897,7 +13017,7 @@
       <c r="N9" s="1"/>
       <c r="O9" s="1"/>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="3" t="str">
         <f t="shared" si="0"/>
         <v>MCVPBirchipCvBaudinTOS13-may</v>
@@ -12930,7 +13050,7 @@
       <c r="N10" s="1"/>
       <c r="O10" s="1"/>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="3" t="str">
         <f t="shared" si="0"/>
         <v>MCVPBirchipCvBulokeTOS13-may</v>
@@ -12963,7 +13083,7 @@
       <c r="N11" s="1"/>
       <c r="O11" s="1"/>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="3" t="str">
         <f t="shared" si="0"/>
         <v>MCVPBirchipCvCapstanTOS13-may</v>
@@ -12996,7 +13116,7 @@
       <c r="N12" s="1"/>
       <c r="O12" s="1"/>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="3" t="str">
         <f t="shared" si="0"/>
         <v>MCVPBirchipCvCommanderTOS13-may</v>
@@ -13029,7 +13149,7 @@
       <c r="N13" s="1"/>
       <c r="O13" s="1"/>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="3" t="str">
         <f t="shared" si="0"/>
         <v>MCVPBirchipCvFleetTOS13-may</v>
@@ -13062,7 +13182,7 @@
       <c r="N14" s="1"/>
       <c r="O14" s="1"/>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="3" t="str">
         <f t="shared" si="0"/>
         <v>MCVPBirchipCvHindmarshTOS13-may</v>
@@ -13095,7 +13215,7 @@
       <c r="N15" s="1"/>
       <c r="O15" s="1"/>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="3" t="str">
         <f t="shared" si="0"/>
         <v>MCVPBirchipCvKeelTOS13-may</v>
@@ -32233,7 +32353,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="705" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="705" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A705" t="s">
         <v>78</v>
       </c>
@@ -32262,7 +32382,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="706" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="706" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A706" t="s">
         <v>79</v>
       </c>
@@ -32291,7 +32411,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="707" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="707" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A707" t="s">
         <v>80</v>
       </c>
@@ -32320,7 +32440,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="708" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="708" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A708" t="s">
         <v>81</v>
       </c>
@@ -32346,7 +32466,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="709" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="709" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A709" t="s">
         <v>82</v>
       </c>
@@ -32372,7 +32492,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="710" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="710" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A710" t="s">
         <v>83</v>
       </c>
@@ -32401,7 +32521,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="711" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="711" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A711" t="s">
         <v>84</v>
       </c>
@@ -32430,7 +32550,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="712" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="712" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A712" t="s">
         <v>85</v>
       </c>
@@ -32459,7 +32579,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="713" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="713" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A713" t="s">
         <v>86</v>
       </c>
@@ -32488,7 +32608,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="714" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="714" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A714" t="s">
         <v>87</v>
       </c>
@@ -32517,7 +32637,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="715" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="715" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A715" t="s">
         <v>88</v>
       </c>
@@ -32543,7 +32663,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="716" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="716" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A716" t="s">
         <v>89</v>
       </c>
@@ -32572,7 +32692,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="717" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="717" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A717" t="s">
         <v>90</v>
       </c>
@@ -32598,7 +32718,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="718" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="718" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A718" t="s">
         <v>91</v>
       </c>
@@ -32622,6 +32742,2854 @@
       </c>
       <c r="K718">
         <v>140</v>
+      </c>
+    </row>
+    <row r="719" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+      <c r="A719" s="18" t="s">
+        <v>118</v>
+      </c>
+      <c r="B719" s="10">
+        <v>33424</v>
+      </c>
+      <c r="C719" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="L719">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="720" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+      <c r="A720" s="18" t="s">
+        <v>118</v>
+      </c>
+      <c r="B720" s="10">
+        <v>33441</v>
+      </c>
+      <c r="C720" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="M720">
+        <v>119.51600000000001</v>
+      </c>
+      <c r="N720">
+        <v>1.044</v>
+      </c>
+      <c r="O720">
+        <v>4.2</v>
+      </c>
+      <c r="P720">
+        <v>0.08</v>
+      </c>
+      <c r="Q720">
+        <v>18</v>
+      </c>
+      <c r="R720">
+        <v>0</v>
+      </c>
+      <c r="T720">
+        <v>3.12</v>
+      </c>
+      <c r="U720">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="721" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+      <c r="A721" s="18" t="s">
+        <v>118</v>
+      </c>
+      <c r="B721" s="10">
+        <v>33455</v>
+      </c>
+      <c r="C721" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="L721">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="722" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+      <c r="A722" s="18" t="s">
+        <v>118</v>
+      </c>
+      <c r="B722" s="10">
+        <v>33456</v>
+      </c>
+      <c r="C722" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="M722">
+        <v>85.770499999999998</v>
+      </c>
+      <c r="N722">
+        <v>1.8285</v>
+      </c>
+      <c r="O722">
+        <v>8</v>
+      </c>
+      <c r="P722">
+        <v>0.19</v>
+      </c>
+      <c r="Q722">
+        <v>23.25</v>
+      </c>
+      <c r="R722">
+        <v>0</v>
+      </c>
+      <c r="T722">
+        <v>6.1565000000000003</v>
+      </c>
+      <c r="U722">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="723" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+      <c r="A723" s="18" t="s">
+        <v>118</v>
+      </c>
+      <c r="B723" s="10">
+        <v>33483</v>
+      </c>
+      <c r="C723" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="M723">
+        <v>99.831500000000005</v>
+      </c>
+      <c r="N723">
+        <v>20.332999999999998</v>
+      </c>
+      <c r="O723">
+        <v>65.45</v>
+      </c>
+      <c r="P723">
+        <v>0.85</v>
+      </c>
+      <c r="Q723">
+        <v>35.5</v>
+      </c>
+      <c r="R723">
+        <v>0</v>
+      </c>
+      <c r="T723">
+        <v>43.781999999999996</v>
+      </c>
+      <c r="U723">
+        <v>1.3014999999999999</v>
+      </c>
+    </row>
+    <row r="724" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+      <c r="A724" s="18" t="s">
+        <v>118</v>
+      </c>
+      <c r="B724" s="10">
+        <v>33504</v>
+      </c>
+      <c r="C724" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="M724">
+        <v>91.39500000000001</v>
+      </c>
+      <c r="N724">
+        <v>85.426999999999992</v>
+      </c>
+      <c r="O724">
+        <v>152.4</v>
+      </c>
+      <c r="P724">
+        <v>1.2549999999999999</v>
+      </c>
+      <c r="Q724">
+        <v>47</v>
+      </c>
+      <c r="R724">
+        <v>1.5190000000000001</v>
+      </c>
+      <c r="S724">
+        <v>0</v>
+      </c>
+      <c r="T724">
+        <v>59.168999999999997</v>
+      </c>
+      <c r="U724">
+        <v>6.0295000000000005</v>
+      </c>
+    </row>
+    <row r="725" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+      <c r="A725" s="18" t="s">
+        <v>118</v>
+      </c>
+      <c r="B725" s="10">
+        <v>33510</v>
+      </c>
+      <c r="C725" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="L725">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="726" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+      <c r="A726" s="18" t="s">
+        <v>118</v>
+      </c>
+      <c r="B726" s="10">
+        <v>33512</v>
+      </c>
+      <c r="C726" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="M726">
+        <v>99.830999999999989</v>
+      </c>
+      <c r="N726">
+        <v>161.07900000000001</v>
+      </c>
+      <c r="O726">
+        <v>288.35000000000002</v>
+      </c>
+      <c r="P726">
+        <v>1.2250000000000001</v>
+      </c>
+      <c r="Q726">
+        <v>49</v>
+      </c>
+      <c r="R726">
+        <v>42.721499999999999</v>
+      </c>
+      <c r="S726">
+        <v>0</v>
+      </c>
+      <c r="T726">
+        <v>58.881500000000003</v>
+      </c>
+      <c r="U726">
+        <v>20.806999999999999</v>
+      </c>
+    </row>
+    <row r="727" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+      <c r="A727" s="18" t="s">
+        <v>118</v>
+      </c>
+      <c r="B727" s="10">
+        <v>33518</v>
+      </c>
+      <c r="C727" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="M727">
+        <v>88.58250000000001</v>
+      </c>
+      <c r="N727">
+        <v>200.76650000000001</v>
+      </c>
+      <c r="O727">
+        <v>397.79999999999995</v>
+      </c>
+      <c r="P727">
+        <v>0.94500000000000006</v>
+      </c>
+      <c r="Q727">
+        <v>42</v>
+      </c>
+      <c r="R727">
+        <v>103.82250000000001</v>
+      </c>
+      <c r="S727">
+        <v>369.79750000000001</v>
+      </c>
+      <c r="T727">
+        <v>51.707999999999998</v>
+      </c>
+      <c r="U727">
+        <v>47.0015</v>
+      </c>
+    </row>
+    <row r="728" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+      <c r="A728" s="18" t="s">
+        <v>118</v>
+      </c>
+      <c r="B728" s="10">
+        <v>33525</v>
+      </c>
+      <c r="C728" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="M728">
+        <v>95.613</v>
+      </c>
+      <c r="N728">
+        <v>125.47800000000001</v>
+      </c>
+      <c r="O728">
+        <v>266.70000000000005</v>
+      </c>
+      <c r="P728">
+        <v>0.215</v>
+      </c>
+      <c r="Q728">
+        <v>41.5</v>
+      </c>
+      <c r="R728">
+        <v>75.390999999999991</v>
+      </c>
+      <c r="S728">
+        <v>312.14850000000001</v>
+      </c>
+      <c r="T728">
+        <v>13.367000000000001</v>
+      </c>
+      <c r="U728">
+        <v>45.422499999999999</v>
+      </c>
+    </row>
+    <row r="729" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+      <c r="A729" s="18" t="s">
+        <v>118</v>
+      </c>
+      <c r="B729" s="10">
+        <v>33532</v>
+      </c>
+      <c r="C729" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="M729">
+        <v>101.23699999999999</v>
+      </c>
+      <c r="N729">
+        <v>139.9495</v>
+      </c>
+      <c r="O729">
+        <v>353.75</v>
+      </c>
+      <c r="P729">
+        <v>0.14500000000000002</v>
+      </c>
+      <c r="Q729">
+        <v>41.5</v>
+      </c>
+      <c r="R729">
+        <v>117.47749999999999</v>
+      </c>
+      <c r="S729">
+        <v>307.93</v>
+      </c>
+      <c r="T729">
+        <v>10.420500000000001</v>
+      </c>
+      <c r="U729">
+        <v>53.723500000000001</v>
+      </c>
+    </row>
+    <row r="730" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+      <c r="A730" s="18" t="s">
+        <v>118</v>
+      </c>
+      <c r="B730" s="10">
+        <v>33539</v>
+      </c>
+      <c r="C730" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="M730">
+        <v>98.425000000000011</v>
+      </c>
+      <c r="N730">
+        <v>118.953</v>
+      </c>
+      <c r="O730">
+        <v>334.3</v>
+      </c>
+      <c r="P730">
+        <v>0</v>
+      </c>
+      <c r="Q730">
+        <v>25.5</v>
+      </c>
+      <c r="R730">
+        <v>138.386</v>
+      </c>
+      <c r="S730">
+        <v>291.0575</v>
+      </c>
+      <c r="T730">
+        <v>8.7499999999999994E-2</v>
+      </c>
+      <c r="U730">
+        <v>60.057499999999997</v>
+      </c>
+    </row>
+    <row r="731" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+      <c r="A731" s="18" t="s">
+        <v>118</v>
+      </c>
+      <c r="B731" s="10">
+        <v>33546</v>
+      </c>
+      <c r="C731" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="M731">
+        <v>104.04949999999999</v>
+      </c>
+      <c r="O731">
+        <v>527.95000000000005</v>
+      </c>
+      <c r="P731">
+        <v>0</v>
+      </c>
+      <c r="Q731">
+        <v>0</v>
+      </c>
+      <c r="R731">
+        <v>251.25900000000001</v>
+      </c>
+      <c r="S731">
+        <v>400.73099999999999</v>
+      </c>
+      <c r="T731">
+        <v>0</v>
+      </c>
+      <c r="U731">
+        <v>54.483000000000004</v>
+      </c>
+    </row>
+    <row r="732" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+      <c r="A732" s="18" t="s">
+        <v>118</v>
+      </c>
+      <c r="B732" s="10">
+        <v>33553</v>
+      </c>
+      <c r="C732" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="L732">
+        <v>10</v>
+      </c>
+      <c r="M732">
+        <v>99.128500000000003</v>
+      </c>
+      <c r="O732">
+        <v>354</v>
+      </c>
+      <c r="P732">
+        <v>0</v>
+      </c>
+      <c r="S732">
+        <v>194.19299999999998</v>
+      </c>
+      <c r="V732">
+        <v>112.964</v>
+      </c>
+      <c r="W732">
+        <v>3.1253299999999999</v>
+      </c>
+    </row>
+    <row r="733" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+      <c r="A733" s="18" t="s">
+        <v>119</v>
+      </c>
+      <c r="B733" s="10">
+        <v>33424</v>
+      </c>
+      <c r="C733" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="L733">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="734" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+      <c r="A734" s="18" t="s">
+        <v>119</v>
+      </c>
+      <c r="B734" s="10">
+        <v>33441</v>
+      </c>
+      <c r="C734" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="M734">
+        <v>109.67400000000001</v>
+      </c>
+      <c r="N734">
+        <v>0.86249999999999993</v>
+      </c>
+      <c r="O734">
+        <v>3.45</v>
+      </c>
+      <c r="P734">
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="Q734">
+        <v>16.5</v>
+      </c>
+      <c r="R734">
+        <v>0</v>
+      </c>
+      <c r="T734">
+        <v>2.5834999999999999</v>
+      </c>
+      <c r="U734">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="735" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+      <c r="A735" s="18" t="s">
+        <v>119</v>
+      </c>
+      <c r="B735" s="10">
+        <v>33455</v>
+      </c>
+      <c r="C735" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="L735">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="736" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+      <c r="A736" s="18" t="s">
+        <v>119</v>
+      </c>
+      <c r="B736" s="10">
+        <v>33456</v>
+      </c>
+      <c r="C736" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="M736">
+        <v>102.643</v>
+      </c>
+      <c r="N736">
+        <v>2.5505</v>
+      </c>
+      <c r="O736">
+        <v>11.4</v>
+      </c>
+      <c r="P736">
+        <v>0.26</v>
+      </c>
+      <c r="Q736">
+        <v>21.25</v>
+      </c>
+      <c r="R736">
+        <v>0</v>
+      </c>
+      <c r="T736">
+        <v>8.68</v>
+      </c>
+      <c r="U736">
+        <v>0.192</v>
+      </c>
+    </row>
+    <row r="737" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+      <c r="A737" s="18" t="s">
+        <v>119</v>
+      </c>
+      <c r="B737" s="10">
+        <v>33483</v>
+      </c>
+      <c r="C737" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="M737">
+        <v>92.801000000000002</v>
+      </c>
+      <c r="N737">
+        <v>17.5855</v>
+      </c>
+      <c r="O737">
+        <v>60.45</v>
+      </c>
+      <c r="P737">
+        <v>0.81</v>
+      </c>
+      <c r="Q737">
+        <v>33.5</v>
+      </c>
+      <c r="R737">
+        <v>0.33850000000000002</v>
+      </c>
+      <c r="T737">
+        <v>40.289500000000004</v>
+      </c>
+      <c r="U737">
+        <v>1.5880000000000001</v>
+      </c>
+    </row>
+    <row r="738" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+      <c r="A738" s="18" t="s">
+        <v>119</v>
+      </c>
+      <c r="B738" s="10">
+        <v>33504</v>
+      </c>
+      <c r="C738" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="M738">
+        <v>98.424999999999997</v>
+      </c>
+      <c r="N738">
+        <v>78.444500000000005</v>
+      </c>
+      <c r="O738">
+        <v>135.65</v>
+      </c>
+      <c r="P738">
+        <v>1.165</v>
+      </c>
+      <c r="Q738">
+        <v>46</v>
+      </c>
+      <c r="R738">
+        <v>1.056</v>
+      </c>
+      <c r="S738">
+        <v>0</v>
+      </c>
+      <c r="T738">
+        <v>49.438000000000002</v>
+      </c>
+      <c r="U738">
+        <v>6.6165000000000003</v>
+      </c>
+    </row>
+    <row r="739" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+      <c r="A739" s="18" t="s">
+        <v>119</v>
+      </c>
+      <c r="B739" s="10">
+        <v>33511</v>
+      </c>
+      <c r="C739" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="L739">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="740" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+      <c r="A740" s="18" t="s">
+        <v>119</v>
+      </c>
+      <c r="B740" s="10">
+        <v>33512</v>
+      </c>
+      <c r="C740" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="M740">
+        <v>99.830999999999989</v>
+      </c>
+      <c r="N740">
+        <v>116.896</v>
+      </c>
+      <c r="O740">
+        <v>206.89999999999998</v>
+      </c>
+      <c r="P740">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="Q740">
+        <v>48</v>
+      </c>
+      <c r="R740">
+        <v>25.3475</v>
+      </c>
+      <c r="S740">
+        <v>0</v>
+      </c>
+      <c r="T740">
+        <v>55.238</v>
+      </c>
+      <c r="U740">
+        <v>5.4995000000000003</v>
+      </c>
+    </row>
+    <row r="741" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+      <c r="A741" s="18" t="s">
+        <v>119</v>
+      </c>
+      <c r="B741" s="10">
+        <v>33518</v>
+      </c>
+      <c r="C741" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="M741">
+        <v>95.613</v>
+      </c>
+      <c r="N741">
+        <v>179.6515</v>
+      </c>
+      <c r="O741">
+        <v>347.7</v>
+      </c>
+      <c r="P741">
+        <v>1.325</v>
+      </c>
+      <c r="Q741">
+        <v>48</v>
+      </c>
+      <c r="R741">
+        <v>84.25</v>
+      </c>
+      <c r="S741">
+        <v>333.23950000000002</v>
+      </c>
+      <c r="T741">
+        <v>67.912499999999994</v>
+      </c>
+      <c r="U741">
+        <v>9.5234999999999985</v>
+      </c>
+    </row>
+    <row r="742" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+      <c r="A742" s="18" t="s">
+        <v>119</v>
+      </c>
+      <c r="B742" s="10">
+        <v>33525</v>
+      </c>
+      <c r="C742" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="M742">
+        <v>98.424999999999997</v>
+      </c>
+      <c r="N742">
+        <v>190.87700000000001</v>
+      </c>
+      <c r="O742">
+        <v>393.45000000000005</v>
+      </c>
+      <c r="P742">
+        <v>1.5750000000000002</v>
+      </c>
+      <c r="Q742">
+        <v>52</v>
+      </c>
+      <c r="R742">
+        <v>103.7195</v>
+      </c>
+      <c r="S742">
+        <v>352.92450000000002</v>
+      </c>
+      <c r="T742">
+        <v>70.724500000000006</v>
+      </c>
+      <c r="U742">
+        <v>7.0860000000000003</v>
+      </c>
+    </row>
+    <row r="743" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+      <c r="A743" s="18" t="s">
+        <v>119</v>
+      </c>
+      <c r="B743" s="10">
+        <v>33532</v>
+      </c>
+      <c r="C743" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="M743">
+        <v>102.643</v>
+      </c>
+      <c r="N743">
+        <v>265.15300000000002</v>
+      </c>
+      <c r="O743">
+        <v>573.04999999999995</v>
+      </c>
+      <c r="P743">
+        <v>1.8299999999999998</v>
+      </c>
+      <c r="Q743">
+        <v>55</v>
+      </c>
+      <c r="R743">
+        <v>196.553</v>
+      </c>
+      <c r="S743">
+        <v>402.137</v>
+      </c>
+      <c r="T743">
+        <v>74.63900000000001</v>
+      </c>
+      <c r="U743">
+        <v>15.57</v>
+      </c>
+    </row>
+    <row r="744" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+      <c r="A744" s="18" t="s">
+        <v>119</v>
+      </c>
+      <c r="B744" s="10">
+        <v>33539</v>
+      </c>
+      <c r="C744" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="M744">
+        <v>104.04949999999999</v>
+      </c>
+      <c r="N744">
+        <v>259.46899999999999</v>
+      </c>
+      <c r="O744">
+        <v>642.6</v>
+      </c>
+      <c r="P744">
+        <v>1.75</v>
+      </c>
+      <c r="Q744">
+        <v>54.5</v>
+      </c>
+      <c r="R744">
+        <v>263.24549999999999</v>
+      </c>
+      <c r="S744">
+        <v>629.92149999999992</v>
+      </c>
+      <c r="T744">
+        <v>66.998999999999995</v>
+      </c>
+      <c r="U744">
+        <v>28.139499999999998</v>
+      </c>
+    </row>
+    <row r="745" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+      <c r="A745" s="18" t="s">
+        <v>119</v>
+      </c>
+      <c r="B745" s="10">
+        <v>33546</v>
+      </c>
+      <c r="C745" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="M745">
+        <v>94.206999999999994</v>
+      </c>
+      <c r="O745">
+        <v>693.84999999999991</v>
+      </c>
+      <c r="P745">
+        <v>0.64999999999999991</v>
+      </c>
+      <c r="Q745">
+        <v>53</v>
+      </c>
+      <c r="R745">
+        <v>344.84899999999999</v>
+      </c>
+      <c r="S745">
+        <v>604.61200000000008</v>
+      </c>
+      <c r="T745">
+        <v>15.960999999999999</v>
+      </c>
+      <c r="U745">
+        <v>35.964500000000001</v>
+      </c>
+    </row>
+    <row r="746" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+      <c r="A746" s="18" t="s">
+        <v>119</v>
+      </c>
+      <c r="B746" s="10">
+        <v>33553</v>
+      </c>
+      <c r="C746" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="M746">
+        <v>108.2675</v>
+      </c>
+      <c r="O746">
+        <v>846.40000000000009</v>
+      </c>
+      <c r="P746">
+        <v>0.58499999999999996</v>
+      </c>
+      <c r="R746">
+        <v>422.82249999999999</v>
+      </c>
+      <c r="S746">
+        <v>809.899</v>
+      </c>
+      <c r="T746">
+        <v>13.324000000000002</v>
+      </c>
+      <c r="U746">
+        <v>43.388500000000001</v>
+      </c>
+    </row>
+    <row r="747" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+      <c r="A747" s="18" t="s">
+        <v>119</v>
+      </c>
+      <c r="B747" s="10">
+        <v>33562</v>
+      </c>
+      <c r="C747" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="L747">
+        <v>10</v>
+      </c>
+      <c r="M747">
+        <v>108.268</v>
+      </c>
+      <c r="O747">
+        <v>769.05</v>
+      </c>
+      <c r="S747">
+        <v>570.55899999999997</v>
+      </c>
+      <c r="V747">
+        <v>322.73649999999998</v>
+      </c>
+      <c r="W747">
+        <v>3.1957599999999999</v>
+      </c>
+    </row>
+    <row r="748" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+      <c r="A748" s="18" t="s">
+        <v>120</v>
+      </c>
+      <c r="B748" s="10">
+        <v>33424</v>
+      </c>
+      <c r="C748" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="L748">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="749" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+      <c r="A749" s="18" t="s">
+        <v>120</v>
+      </c>
+      <c r="B749" s="10">
+        <v>33441</v>
+      </c>
+      <c r="C749" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="M749">
+        <v>112.48599999999999</v>
+      </c>
+      <c r="N749">
+        <v>0.996</v>
+      </c>
+      <c r="O749">
+        <v>3.7</v>
+      </c>
+      <c r="P749">
+        <v>7.5000000000000011E-2</v>
+      </c>
+      <c r="Q749">
+        <v>17.75</v>
+      </c>
+      <c r="R749">
+        <v>0</v>
+      </c>
+      <c r="T749">
+        <v>2.6924999999999999</v>
+      </c>
+      <c r="U749">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="750" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+      <c r="A750" s="18" t="s">
+        <v>120</v>
+      </c>
+      <c r="B750" s="10">
+        <v>33455</v>
+      </c>
+      <c r="C750" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="L750">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="751" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+      <c r="A751" s="18" t="s">
+        <v>120</v>
+      </c>
+      <c r="B751" s="10">
+        <v>33456</v>
+      </c>
+      <c r="C751" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="M751">
+        <v>95.613</v>
+      </c>
+      <c r="N751">
+        <v>2.5644999999999998</v>
+      </c>
+      <c r="O751">
+        <v>11.55</v>
+      </c>
+      <c r="P751">
+        <v>0.28500000000000003</v>
+      </c>
+      <c r="Q751">
+        <v>28.5</v>
+      </c>
+      <c r="R751">
+        <v>0</v>
+      </c>
+      <c r="T751">
+        <v>8.9789999999999992</v>
+      </c>
+      <c r="U751">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="752" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+      <c r="A752" s="18" t="s">
+        <v>120</v>
+      </c>
+      <c r="B752" s="10">
+        <v>33483</v>
+      </c>
+      <c r="C752" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="M752">
+        <v>91.39500000000001</v>
+      </c>
+      <c r="N752">
+        <v>26.811500000000002</v>
+      </c>
+      <c r="O752">
+        <v>87.9</v>
+      </c>
+      <c r="P752">
+        <v>1.415</v>
+      </c>
+      <c r="Q752">
+        <v>47.5</v>
+      </c>
+      <c r="R752">
+        <v>0</v>
+      </c>
+      <c r="T752">
+        <v>60.523499999999999</v>
+      </c>
+      <c r="U752">
+        <v>0.58850000000000002</v>
+      </c>
+    </row>
+    <row r="753" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+      <c r="A753" s="18" t="s">
+        <v>120</v>
+      </c>
+      <c r="B753" s="10">
+        <v>33504</v>
+      </c>
+      <c r="C753" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="M753">
+        <v>88.582999999999998</v>
+      </c>
+      <c r="N753">
+        <v>169.19150000000002</v>
+      </c>
+      <c r="O753">
+        <v>312.45</v>
+      </c>
+      <c r="P753">
+        <v>4.0049999999999999</v>
+      </c>
+      <c r="Q753">
+        <v>64.5</v>
+      </c>
+      <c r="R753">
+        <v>0.17699999999999999</v>
+      </c>
+      <c r="S753">
+        <v>0</v>
+      </c>
+      <c r="T753">
+        <v>137.321</v>
+      </c>
+      <c r="U753">
+        <v>5.9450000000000003</v>
+      </c>
+    </row>
+    <row r="754" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+      <c r="A754" s="18" t="s">
+        <v>120</v>
+      </c>
+      <c r="B754" s="10">
+        <v>33512</v>
+      </c>
+      <c r="C754" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="M754">
+        <v>92.801000000000002</v>
+      </c>
+      <c r="N754">
+        <v>268.75400000000002</v>
+      </c>
+      <c r="O754">
+        <v>456.8</v>
+      </c>
+      <c r="P754">
+        <v>3.96</v>
+      </c>
+      <c r="Q754">
+        <v>72</v>
+      </c>
+      <c r="R754">
+        <v>32.164500000000004</v>
+      </c>
+      <c r="S754">
+        <v>0</v>
+      </c>
+      <c r="T754">
+        <v>137.80350000000001</v>
+      </c>
+      <c r="U754">
+        <v>13.5395</v>
+      </c>
+    </row>
+    <row r="755" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+      <c r="A755" s="18" t="s">
+        <v>120</v>
+      </c>
+      <c r="B755" s="10">
+        <v>33513</v>
+      </c>
+      <c r="C755" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="L755">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="756" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+      <c r="A756" s="18" t="s">
+        <v>120</v>
+      </c>
+      <c r="B756" s="10">
+        <v>33518</v>
+      </c>
+      <c r="C756" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="M756">
+        <v>89.989000000000004</v>
+      </c>
+      <c r="N756">
+        <v>357.08850000000001</v>
+      </c>
+      <c r="O756">
+        <v>623.90000000000009</v>
+      </c>
+      <c r="P756">
+        <v>3.45</v>
+      </c>
+      <c r="Q756">
+        <v>72</v>
+      </c>
+      <c r="R756">
+        <v>119.4555</v>
+      </c>
+      <c r="S756">
+        <v>352.92449999999997</v>
+      </c>
+      <c r="T756">
+        <v>125.92699999999999</v>
+      </c>
+      <c r="U756">
+        <v>23.974</v>
+      </c>
+    </row>
+    <row r="757" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+      <c r="A757" s="18" t="s">
+        <v>120</v>
+      </c>
+      <c r="B757" s="10">
+        <v>33525</v>
+      </c>
+      <c r="C757" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="M757">
+        <v>95.613</v>
+      </c>
+      <c r="N757">
+        <v>369.73849999999999</v>
+      </c>
+      <c r="O757">
+        <v>694.09999999999991</v>
+      </c>
+      <c r="P757">
+        <v>2.5949999999999998</v>
+      </c>
+      <c r="Q757">
+        <v>76.5</v>
+      </c>
+      <c r="R757">
+        <v>167.85250000000002</v>
+      </c>
+      <c r="S757">
+        <v>385.2645</v>
+      </c>
+      <c r="T757">
+        <v>106.3685</v>
+      </c>
+      <c r="U757">
+        <v>30.823</v>
+      </c>
+    </row>
+    <row r="758" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+      <c r="A758" s="18" t="s">
+        <v>120</v>
+      </c>
+      <c r="B758" s="10">
+        <v>33532</v>
+      </c>
+      <c r="C758" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="M758">
+        <v>94.206999999999994</v>
+      </c>
+      <c r="N758">
+        <v>406.22550000000001</v>
+      </c>
+      <c r="O758">
+        <v>862.40000000000009</v>
+      </c>
+      <c r="P758">
+        <v>2.67</v>
+      </c>
+      <c r="Q758">
+        <v>74</v>
+      </c>
+      <c r="R758">
+        <v>308.3175</v>
+      </c>
+      <c r="S758">
+        <v>469.62900000000002</v>
+      </c>
+      <c r="T758">
+        <v>97.634500000000003</v>
+      </c>
+      <c r="U758">
+        <v>38.8825</v>
+      </c>
+    </row>
+    <row r="759" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+      <c r="A759" s="18" t="s">
+        <v>120</v>
+      </c>
+      <c r="B759" s="10">
+        <v>33539</v>
+      </c>
+      <c r="C759" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="M759">
+        <v>89.989000000000004</v>
+      </c>
+      <c r="N759">
+        <v>404.30599999999998</v>
+      </c>
+      <c r="O759">
+        <v>945.85</v>
+      </c>
+      <c r="P759">
+        <v>1.2850000000000001</v>
+      </c>
+      <c r="Q759">
+        <v>77.5</v>
+      </c>
+      <c r="R759">
+        <v>397.786</v>
+      </c>
+      <c r="S759">
+        <v>427.44650000000001</v>
+      </c>
+      <c r="T759">
+        <v>60.980000000000004</v>
+      </c>
+      <c r="U759">
+        <v>72.403000000000006</v>
+      </c>
+    </row>
+    <row r="760" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+      <c r="A760" s="18" t="s">
+        <v>120</v>
+      </c>
+      <c r="B760" s="10">
+        <v>33546</v>
+      </c>
+      <c r="C760" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="M760">
+        <v>97.019000000000005</v>
+      </c>
+      <c r="O760">
+        <v>1042</v>
+      </c>
+      <c r="P760">
+        <v>0.62</v>
+      </c>
+      <c r="Q760">
+        <v>73.5</v>
+      </c>
+      <c r="R760">
+        <v>509.1345</v>
+      </c>
+      <c r="S760">
+        <v>503.37450000000001</v>
+      </c>
+      <c r="T760">
+        <v>23.896000000000001</v>
+      </c>
+      <c r="U760">
+        <v>95.6935</v>
+      </c>
+    </row>
+    <row r="761" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+      <c r="A761" s="18" t="s">
+        <v>120</v>
+      </c>
+      <c r="B761" s="10">
+        <v>33553</v>
+      </c>
+      <c r="C761" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="M761">
+        <v>94.206999999999994</v>
+      </c>
+      <c r="O761">
+        <v>934.55</v>
+      </c>
+      <c r="P761">
+        <v>0.04</v>
+      </c>
+      <c r="R761">
+        <v>467.82950000000005</v>
+      </c>
+      <c r="S761">
+        <v>466.81650000000002</v>
+      </c>
+      <c r="T761">
+        <v>1.0665</v>
+      </c>
+      <c r="U761">
+        <v>96.275499999999994</v>
+      </c>
+    </row>
+    <row r="762" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+      <c r="A762" s="18" t="s">
+        <v>120</v>
+      </c>
+      <c r="B762" s="10">
+        <v>33560</v>
+      </c>
+      <c r="C762" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="L762">
+        <v>10</v>
+      </c>
+      <c r="M762">
+        <v>97.019000000000005</v>
+      </c>
+      <c r="O762">
+        <v>1049.5</v>
+      </c>
+      <c r="S762">
+        <v>400.35699999999997</v>
+      </c>
+      <c r="V762">
+        <v>431.13049999999998</v>
+      </c>
+      <c r="W762">
+        <v>4.2832699999999999</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F84229A8-208F-47CC-9C04-F24716D32173}">
+  <dimension ref="A1:N45"/>
+  <sheetViews>
+    <sheetView topLeftCell="C39" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:N45"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="2" max="2" width="9.05078125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.15625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.68359375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.68359375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>102</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="E1" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="F1" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="G1" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="H1" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="I1" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="J1" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="K1" s="14" t="s">
+        <v>110</v>
+      </c>
+      <c r="L1" s="14" t="s">
+        <v>111</v>
+      </c>
+      <c r="M1" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="N1" s="14" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="15" t="s">
+        <v>114</v>
+      </c>
+      <c r="B2" s="17">
+        <v>33424</v>
+      </c>
+      <c r="C2" s="9">
+        <v>3</v>
+      </c>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="9"/>
+      <c r="L2" s="9"/>
+      <c r="M2" s="9"/>
+      <c r="N2" s="9"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="15"/>
+      <c r="B3" s="11">
+        <v>33441</v>
+      </c>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9">
+        <v>119.51600000000001</v>
+      </c>
+      <c r="E3" s="9">
+        <v>1.044</v>
+      </c>
+      <c r="F3" s="9">
+        <v>4.2</v>
+      </c>
+      <c r="G3" s="9">
+        <v>0.08</v>
+      </c>
+      <c r="H3" s="9">
+        <v>18</v>
+      </c>
+      <c r="I3" s="9">
+        <v>0</v>
+      </c>
+      <c r="J3" s="9"/>
+      <c r="K3" s="9">
+        <v>3.12</v>
+      </c>
+      <c r="L3" s="9">
+        <v>0</v>
+      </c>
+      <c r="M3" s="9"/>
+      <c r="N3" s="9"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="15"/>
+      <c r="B4" s="11">
+        <v>33455</v>
+      </c>
+      <c r="C4" s="9">
+        <v>5</v>
+      </c>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="9"/>
+      <c r="K4" s="9"/>
+      <c r="L4" s="9"/>
+      <c r="M4" s="9"/>
+      <c r="N4" s="9"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="15"/>
+      <c r="B5" s="11">
+        <v>33456</v>
+      </c>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9">
+        <v>85.770499999999998</v>
+      </c>
+      <c r="E5" s="9">
+        <v>1.8285</v>
+      </c>
+      <c r="F5" s="9">
+        <v>8</v>
+      </c>
+      <c r="G5" s="9">
+        <v>0.19</v>
+      </c>
+      <c r="H5" s="9">
+        <v>23.25</v>
+      </c>
+      <c r="I5" s="9">
+        <v>0</v>
+      </c>
+      <c r="J5" s="9"/>
+      <c r="K5" s="9">
+        <v>6.1565000000000003</v>
+      </c>
+      <c r="L5" s="9">
+        <v>0</v>
+      </c>
+      <c r="M5" s="9"/>
+      <c r="N5" s="9"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" s="15"/>
+      <c r="B6" s="11">
+        <v>33483</v>
+      </c>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9">
+        <v>99.831500000000005</v>
+      </c>
+      <c r="E6" s="9">
+        <v>20.332999999999998</v>
+      </c>
+      <c r="F6" s="9">
+        <v>65.45</v>
+      </c>
+      <c r="G6" s="9">
+        <v>0.85</v>
+      </c>
+      <c r="H6" s="9">
+        <v>35.5</v>
+      </c>
+      <c r="I6" s="9">
+        <v>0</v>
+      </c>
+      <c r="J6" s="9"/>
+      <c r="K6" s="9">
+        <v>43.781999999999996</v>
+      </c>
+      <c r="L6" s="9">
+        <v>1.3014999999999999</v>
+      </c>
+      <c r="M6" s="9"/>
+      <c r="N6" s="9"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" s="15"/>
+      <c r="B7" s="11">
+        <v>33504</v>
+      </c>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9">
+        <v>91.39500000000001</v>
+      </c>
+      <c r="E7" s="9">
+        <v>85.426999999999992</v>
+      </c>
+      <c r="F7" s="9">
+        <v>152.4</v>
+      </c>
+      <c r="G7" s="9">
+        <v>1.2549999999999999</v>
+      </c>
+      <c r="H7" s="9">
+        <v>47</v>
+      </c>
+      <c r="I7" s="9">
+        <v>1.5190000000000001</v>
+      </c>
+      <c r="J7" s="9">
+        <v>0</v>
+      </c>
+      <c r="K7" s="9">
+        <v>59.168999999999997</v>
+      </c>
+      <c r="L7" s="9">
+        <v>6.0295000000000005</v>
+      </c>
+      <c r="M7" s="9"/>
+      <c r="N7" s="9"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" s="15"/>
+      <c r="B8" s="11">
+        <v>33510</v>
+      </c>
+      <c r="C8" s="9">
+        <v>7</v>
+      </c>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="9"/>
+      <c r="K8" s="9"/>
+      <c r="L8" s="9"/>
+      <c r="M8" s="9"/>
+      <c r="N8" s="9"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" s="15"/>
+      <c r="B9" s="11">
+        <v>33512</v>
+      </c>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9">
+        <v>99.830999999999989</v>
+      </c>
+      <c r="E9" s="9">
+        <v>161.07900000000001</v>
+      </c>
+      <c r="F9" s="9">
+        <v>288.35000000000002</v>
+      </c>
+      <c r="G9" s="9">
+        <v>1.2250000000000001</v>
+      </c>
+      <c r="H9" s="9">
+        <v>49</v>
+      </c>
+      <c r="I9" s="9">
+        <v>42.721499999999999</v>
+      </c>
+      <c r="J9" s="9">
+        <v>0</v>
+      </c>
+      <c r="K9" s="9">
+        <v>58.881500000000003</v>
+      </c>
+      <c r="L9" s="9">
+        <v>20.806999999999999</v>
+      </c>
+      <c r="M9" s="9"/>
+      <c r="N9" s="9"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" s="15"/>
+      <c r="B10" s="11">
+        <v>33518</v>
+      </c>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9">
+        <v>88.58250000000001</v>
+      </c>
+      <c r="E10" s="9">
+        <v>200.76650000000001</v>
+      </c>
+      <c r="F10" s="9">
+        <v>397.79999999999995</v>
+      </c>
+      <c r="G10" s="9">
+        <v>0.94500000000000006</v>
+      </c>
+      <c r="H10" s="9">
+        <v>42</v>
+      </c>
+      <c r="I10" s="9">
+        <v>103.82250000000001</v>
+      </c>
+      <c r="J10" s="9">
+        <v>369.79750000000001</v>
+      </c>
+      <c r="K10" s="9">
+        <v>51.707999999999998</v>
+      </c>
+      <c r="L10" s="9">
+        <v>47.0015</v>
+      </c>
+      <c r="M10" s="9"/>
+      <c r="N10" s="9"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" s="15"/>
+      <c r="B11" s="11">
+        <v>33525</v>
+      </c>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9">
+        <v>95.613</v>
+      </c>
+      <c r="E11" s="9">
+        <v>125.47800000000001</v>
+      </c>
+      <c r="F11" s="9">
+        <v>266.70000000000005</v>
+      </c>
+      <c r="G11" s="9">
+        <v>0.215</v>
+      </c>
+      <c r="H11" s="9">
+        <v>41.5</v>
+      </c>
+      <c r="I11" s="9">
+        <v>75.390999999999991</v>
+      </c>
+      <c r="J11" s="9">
+        <v>312.14850000000001</v>
+      </c>
+      <c r="K11" s="9">
+        <v>13.367000000000001</v>
+      </c>
+      <c r="L11" s="9">
+        <v>45.422499999999999</v>
+      </c>
+      <c r="M11" s="9"/>
+      <c r="N11" s="9"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" s="15"/>
+      <c r="B12" s="11">
+        <v>33532</v>
+      </c>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9">
+        <v>101.23699999999999</v>
+      </c>
+      <c r="E12" s="9">
+        <v>139.9495</v>
+      </c>
+      <c r="F12" s="9">
+        <v>353.75</v>
+      </c>
+      <c r="G12" s="9">
+        <v>0.14500000000000002</v>
+      </c>
+      <c r="H12" s="9">
+        <v>41.5</v>
+      </c>
+      <c r="I12" s="9">
+        <v>117.47749999999999</v>
+      </c>
+      <c r="J12" s="9">
+        <v>307.93</v>
+      </c>
+      <c r="K12" s="9">
+        <v>10.420500000000001</v>
+      </c>
+      <c r="L12" s="9">
+        <v>53.723500000000001</v>
+      </c>
+      <c r="M12" s="9"/>
+      <c r="N12" s="9"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" s="15"/>
+      <c r="B13" s="11">
+        <v>33539</v>
+      </c>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9">
+        <v>98.425000000000011</v>
+      </c>
+      <c r="E13" s="9">
+        <v>118.953</v>
+      </c>
+      <c r="F13" s="9">
+        <v>334.3</v>
+      </c>
+      <c r="G13" s="9">
+        <v>0</v>
+      </c>
+      <c r="H13" s="9">
+        <v>25.5</v>
+      </c>
+      <c r="I13" s="9">
+        <v>138.386</v>
+      </c>
+      <c r="J13" s="9">
+        <v>291.0575</v>
+      </c>
+      <c r="K13" s="9">
+        <v>8.7499999999999994E-2</v>
+      </c>
+      <c r="L13" s="9">
+        <v>60.057499999999997</v>
+      </c>
+      <c r="M13" s="9"/>
+      <c r="N13" s="9"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" s="15"/>
+      <c r="B14" s="11">
+        <v>33546</v>
+      </c>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9">
+        <v>104.04949999999999</v>
+      </c>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9">
+        <v>527.95000000000005</v>
+      </c>
+      <c r="G14" s="9">
+        <v>0</v>
+      </c>
+      <c r="H14" s="9">
+        <v>0</v>
+      </c>
+      <c r="I14" s="9">
+        <v>251.25900000000001</v>
+      </c>
+      <c r="J14" s="9">
+        <v>400.73099999999999</v>
+      </c>
+      <c r="K14" s="9">
+        <v>0</v>
+      </c>
+      <c r="L14" s="9">
+        <v>54.483000000000004</v>
+      </c>
+      <c r="M14" s="9"/>
+      <c r="N14" s="9"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" s="16"/>
+      <c r="B15" s="11">
+        <v>33553</v>
+      </c>
+      <c r="C15" s="9">
+        <v>10</v>
+      </c>
+      <c r="D15" s="9">
+        <v>99.128500000000003</v>
+      </c>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9">
+        <v>354</v>
+      </c>
+      <c r="G15" s="9">
+        <v>0</v>
+      </c>
+      <c r="H15" s="9"/>
+      <c r="I15" s="9"/>
+      <c r="J15" s="9">
+        <v>194.19299999999998</v>
+      </c>
+      <c r="K15" s="9"/>
+      <c r="L15" s="9"/>
+      <c r="M15" s="9">
+        <v>112.964</v>
+      </c>
+      <c r="N15" s="9">
+        <v>3.1253299999999999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="B16" s="11">
+        <v>33424</v>
+      </c>
+      <c r="C16" s="9">
+        <v>3</v>
+      </c>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="9"/>
+      <c r="G16" s="9"/>
+      <c r="H16" s="9"/>
+      <c r="I16" s="9"/>
+      <c r="J16" s="9"/>
+      <c r="K16" s="9"/>
+      <c r="L16" s="9"/>
+      <c r="M16" s="9"/>
+      <c r="N16" s="9"/>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" s="15"/>
+      <c r="B17" s="11">
+        <v>33441</v>
+      </c>
+      <c r="C17" s="9"/>
+      <c r="D17" s="9">
+        <v>109.67400000000001</v>
+      </c>
+      <c r="E17" s="9">
+        <v>0.86249999999999993</v>
+      </c>
+      <c r="F17" s="9">
+        <v>3.45</v>
+      </c>
+      <c r="G17" s="9">
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="H17" s="9">
+        <v>16.5</v>
+      </c>
+      <c r="I17" s="9">
+        <v>0</v>
+      </c>
+      <c r="J17" s="9"/>
+      <c r="K17" s="9">
+        <v>2.5834999999999999</v>
+      </c>
+      <c r="L17" s="9">
+        <v>0</v>
+      </c>
+      <c r="M17" s="9"/>
+      <c r="N17" s="9"/>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18" s="15"/>
+      <c r="B18" s="11">
+        <v>33455</v>
+      </c>
+      <c r="C18" s="9">
+        <v>5</v>
+      </c>
+      <c r="D18" s="9"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="9"/>
+      <c r="G18" s="9"/>
+      <c r="H18" s="9"/>
+      <c r="I18" s="9"/>
+      <c r="J18" s="9"/>
+      <c r="K18" s="9"/>
+      <c r="L18" s="9"/>
+      <c r="M18" s="9"/>
+      <c r="N18" s="9"/>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19" s="15"/>
+      <c r="B19" s="11">
+        <v>33456</v>
+      </c>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9">
+        <v>102.643</v>
+      </c>
+      <c r="E19" s="9">
+        <v>2.5505</v>
+      </c>
+      <c r="F19" s="9">
+        <v>11.4</v>
+      </c>
+      <c r="G19" s="9">
+        <v>0.26</v>
+      </c>
+      <c r="H19" s="9">
+        <v>21.25</v>
+      </c>
+      <c r="I19" s="9">
+        <v>0</v>
+      </c>
+      <c r="J19" s="9"/>
+      <c r="K19" s="9">
+        <v>8.68</v>
+      </c>
+      <c r="L19" s="9">
+        <v>0.192</v>
+      </c>
+      <c r="M19" s="9"/>
+      <c r="N19" s="9"/>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20" s="15"/>
+      <c r="B20" s="11">
+        <v>33483</v>
+      </c>
+      <c r="C20" s="9"/>
+      <c r="D20" s="9">
+        <v>92.801000000000002</v>
+      </c>
+      <c r="E20" s="9">
+        <v>17.5855</v>
+      </c>
+      <c r="F20" s="9">
+        <v>60.45</v>
+      </c>
+      <c r="G20" s="9">
+        <v>0.81</v>
+      </c>
+      <c r="H20" s="9">
+        <v>33.5</v>
+      </c>
+      <c r="I20" s="9">
+        <v>0.33850000000000002</v>
+      </c>
+      <c r="J20" s="9"/>
+      <c r="K20" s="9">
+        <v>40.289500000000004</v>
+      </c>
+      <c r="L20" s="9">
+        <v>1.5880000000000001</v>
+      </c>
+      <c r="M20" s="9"/>
+      <c r="N20" s="9"/>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21" s="15"/>
+      <c r="B21" s="11">
+        <v>33504</v>
+      </c>
+      <c r="C21" s="9"/>
+      <c r="D21" s="9">
+        <v>98.424999999999997</v>
+      </c>
+      <c r="E21" s="9">
+        <v>78.444500000000005</v>
+      </c>
+      <c r="F21" s="9">
+        <v>135.65</v>
+      </c>
+      <c r="G21" s="9">
+        <v>1.165</v>
+      </c>
+      <c r="H21" s="9">
+        <v>46</v>
+      </c>
+      <c r="I21" s="9">
+        <v>1.056</v>
+      </c>
+      <c r="J21" s="9">
+        <v>0</v>
+      </c>
+      <c r="K21" s="9">
+        <v>49.438000000000002</v>
+      </c>
+      <c r="L21" s="9">
+        <v>6.6165000000000003</v>
+      </c>
+      <c r="M21" s="9"/>
+      <c r="N21" s="9"/>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A22" s="15"/>
+      <c r="B22" s="11">
+        <v>33511</v>
+      </c>
+      <c r="C22" s="9">
+        <v>7</v>
+      </c>
+      <c r="D22" s="9"/>
+      <c r="E22" s="9"/>
+      <c r="F22" s="9"/>
+      <c r="G22" s="9"/>
+      <c r="H22" s="9"/>
+      <c r="I22" s="9"/>
+      <c r="J22" s="9"/>
+      <c r="K22" s="9"/>
+      <c r="L22" s="9"/>
+      <c r="M22" s="9"/>
+      <c r="N22" s="9"/>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A23" s="15"/>
+      <c r="B23" s="11">
+        <v>33512</v>
+      </c>
+      <c r="C23" s="9"/>
+      <c r="D23" s="9">
+        <v>99.830999999999989</v>
+      </c>
+      <c r="E23" s="9">
+        <v>116.896</v>
+      </c>
+      <c r="F23" s="9">
+        <v>206.89999999999998</v>
+      </c>
+      <c r="G23" s="9">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="H23" s="9">
+        <v>48</v>
+      </c>
+      <c r="I23" s="9">
+        <v>25.3475</v>
+      </c>
+      <c r="J23" s="9">
+        <v>0</v>
+      </c>
+      <c r="K23" s="9">
+        <v>55.238</v>
+      </c>
+      <c r="L23" s="9">
+        <v>5.4995000000000003</v>
+      </c>
+      <c r="M23" s="9"/>
+      <c r="N23" s="9"/>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A24" s="15"/>
+      <c r="B24" s="11">
+        <v>33518</v>
+      </c>
+      <c r="C24" s="9"/>
+      <c r="D24" s="9">
+        <v>95.613</v>
+      </c>
+      <c r="E24" s="9">
+        <v>179.6515</v>
+      </c>
+      <c r="F24" s="9">
+        <v>347.7</v>
+      </c>
+      <c r="G24" s="9">
+        <v>1.325</v>
+      </c>
+      <c r="H24" s="9">
+        <v>48</v>
+      </c>
+      <c r="I24" s="9">
+        <v>84.25</v>
+      </c>
+      <c r="J24" s="9">
+        <v>333.23950000000002</v>
+      </c>
+      <c r="K24" s="9">
+        <v>67.912499999999994</v>
+      </c>
+      <c r="L24" s="9">
+        <v>9.5234999999999985</v>
+      </c>
+      <c r="M24" s="9"/>
+      <c r="N24" s="9"/>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A25" s="15"/>
+      <c r="B25" s="11">
+        <v>33525</v>
+      </c>
+      <c r="C25" s="9"/>
+      <c r="D25" s="9">
+        <v>98.424999999999997</v>
+      </c>
+      <c r="E25" s="9">
+        <v>190.87700000000001</v>
+      </c>
+      <c r="F25" s="9">
+        <v>393.45000000000005</v>
+      </c>
+      <c r="G25" s="9">
+        <v>1.5750000000000002</v>
+      </c>
+      <c r="H25" s="9">
+        <v>52</v>
+      </c>
+      <c r="I25" s="9">
+        <v>103.7195</v>
+      </c>
+      <c r="J25" s="9">
+        <v>352.92450000000002</v>
+      </c>
+      <c r="K25" s="9">
+        <v>70.724500000000006</v>
+      </c>
+      <c r="L25" s="9">
+        <v>7.0860000000000003</v>
+      </c>
+      <c r="M25" s="9"/>
+      <c r="N25" s="9"/>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A26" s="15"/>
+      <c r="B26" s="11">
+        <v>33532</v>
+      </c>
+      <c r="C26" s="9"/>
+      <c r="D26" s="9">
+        <v>102.643</v>
+      </c>
+      <c r="E26" s="9">
+        <v>265.15300000000002</v>
+      </c>
+      <c r="F26" s="9">
+        <v>573.04999999999995</v>
+      </c>
+      <c r="G26" s="9">
+        <v>1.8299999999999998</v>
+      </c>
+      <c r="H26" s="9">
+        <v>55</v>
+      </c>
+      <c r="I26" s="9">
+        <v>196.553</v>
+      </c>
+      <c r="J26" s="9">
+        <v>402.137</v>
+      </c>
+      <c r="K26" s="9">
+        <v>74.63900000000001</v>
+      </c>
+      <c r="L26" s="9">
+        <v>15.57</v>
+      </c>
+      <c r="M26" s="9"/>
+      <c r="N26" s="9"/>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A27" s="15"/>
+      <c r="B27" s="11">
+        <v>33539</v>
+      </c>
+      <c r="C27" s="9"/>
+      <c r="D27" s="9">
+        <v>104.04949999999999</v>
+      </c>
+      <c r="E27" s="9">
+        <v>259.46899999999999</v>
+      </c>
+      <c r="F27" s="9">
+        <v>642.6</v>
+      </c>
+      <c r="G27" s="9">
+        <v>1.75</v>
+      </c>
+      <c r="H27" s="9">
+        <v>54.5</v>
+      </c>
+      <c r="I27" s="9">
+        <v>263.24549999999999</v>
+      </c>
+      <c r="J27" s="9">
+        <v>629.92149999999992</v>
+      </c>
+      <c r="K27" s="9">
+        <v>66.998999999999995</v>
+      </c>
+      <c r="L27" s="9">
+        <v>28.139499999999998</v>
+      </c>
+      <c r="M27" s="9"/>
+      <c r="N27" s="9"/>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A28" s="15"/>
+      <c r="B28" s="11">
+        <v>33546</v>
+      </c>
+      <c r="C28" s="9"/>
+      <c r="D28" s="9">
+        <v>94.206999999999994</v>
+      </c>
+      <c r="E28" s="9"/>
+      <c r="F28" s="9">
+        <v>693.84999999999991</v>
+      </c>
+      <c r="G28" s="9">
+        <v>0.64999999999999991</v>
+      </c>
+      <c r="H28" s="9">
+        <v>53</v>
+      </c>
+      <c r="I28" s="9">
+        <v>344.84899999999999</v>
+      </c>
+      <c r="J28" s="9">
+        <v>604.61200000000008</v>
+      </c>
+      <c r="K28" s="9">
+        <v>15.960999999999999</v>
+      </c>
+      <c r="L28" s="9">
+        <v>35.964500000000001</v>
+      </c>
+      <c r="M28" s="9"/>
+      <c r="N28" s="9"/>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A29" s="15"/>
+      <c r="B29" s="11">
+        <v>33553</v>
+      </c>
+      <c r="C29" s="9"/>
+      <c r="D29" s="9">
+        <v>108.2675</v>
+      </c>
+      <c r="E29" s="9"/>
+      <c r="F29" s="9">
+        <v>846.40000000000009</v>
+      </c>
+      <c r="G29" s="9">
+        <v>0.58499999999999996</v>
+      </c>
+      <c r="H29" s="9"/>
+      <c r="I29" s="9">
+        <v>422.82249999999999</v>
+      </c>
+      <c r="J29" s="9">
+        <v>809.899</v>
+      </c>
+      <c r="K29" s="9">
+        <v>13.324000000000002</v>
+      </c>
+      <c r="L29" s="9">
+        <v>43.388500000000001</v>
+      </c>
+      <c r="M29" s="9"/>
+      <c r="N29" s="9"/>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A30" s="16"/>
+      <c r="B30" s="11">
+        <v>33562</v>
+      </c>
+      <c r="C30" s="9">
+        <v>10</v>
+      </c>
+      <c r="D30" s="9">
+        <v>108.268</v>
+      </c>
+      <c r="E30" s="9"/>
+      <c r="F30" s="9">
+        <v>769.05</v>
+      </c>
+      <c r="G30" s="9"/>
+      <c r="H30" s="9"/>
+      <c r="I30" s="9"/>
+      <c r="J30" s="9">
+        <v>570.55899999999997</v>
+      </c>
+      <c r="K30" s="9"/>
+      <c r="L30" s="9"/>
+      <c r="M30" s="9">
+        <v>322.73649999999998</v>
+      </c>
+      <c r="N30" s="9">
+        <v>3.1957599999999999</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A31" s="15" t="s">
+        <v>116</v>
+      </c>
+      <c r="B31" s="11">
+        <v>33424</v>
+      </c>
+      <c r="C31" s="9">
+        <v>3</v>
+      </c>
+      <c r="D31" s="9"/>
+      <c r="E31" s="9"/>
+      <c r="F31" s="9"/>
+      <c r="G31" s="9"/>
+      <c r="H31" s="9"/>
+      <c r="I31" s="9"/>
+      <c r="J31" s="9"/>
+      <c r="K31" s="9"/>
+      <c r="L31" s="9"/>
+      <c r="M31" s="9"/>
+      <c r="N31" s="9"/>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A32" s="15"/>
+      <c r="B32" s="11">
+        <v>33441</v>
+      </c>
+      <c r="C32" s="9"/>
+      <c r="D32" s="9">
+        <v>112.48599999999999</v>
+      </c>
+      <c r="E32" s="9">
+        <v>0.996</v>
+      </c>
+      <c r="F32" s="9">
+        <v>3.7</v>
+      </c>
+      <c r="G32" s="9">
+        <v>7.5000000000000011E-2</v>
+      </c>
+      <c r="H32" s="9">
+        <v>17.75</v>
+      </c>
+      <c r="I32" s="9">
+        <v>0</v>
+      </c>
+      <c r="J32" s="9"/>
+      <c r="K32" s="9">
+        <v>2.6924999999999999</v>
+      </c>
+      <c r="L32" s="9">
+        <v>0</v>
+      </c>
+      <c r="M32" s="9"/>
+      <c r="N32" s="9"/>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A33" s="15"/>
+      <c r="B33" s="11">
+        <v>33455</v>
+      </c>
+      <c r="C33" s="9">
+        <v>5</v>
+      </c>
+      <c r="D33" s="9"/>
+      <c r="E33" s="9"/>
+      <c r="F33" s="9"/>
+      <c r="G33" s="9"/>
+      <c r="H33" s="9"/>
+      <c r="I33" s="9"/>
+      <c r="J33" s="9"/>
+      <c r="K33" s="9"/>
+      <c r="L33" s="9"/>
+      <c r="M33" s="9"/>
+      <c r="N33" s="9"/>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A34" s="15"/>
+      <c r="B34" s="11">
+        <v>33456</v>
+      </c>
+      <c r="C34" s="9"/>
+      <c r="D34" s="9">
+        <v>95.613</v>
+      </c>
+      <c r="E34" s="9">
+        <v>2.5644999999999998</v>
+      </c>
+      <c r="F34" s="9">
+        <v>11.55</v>
+      </c>
+      <c r="G34" s="9">
+        <v>0.28500000000000003</v>
+      </c>
+      <c r="H34" s="9">
+        <v>28.5</v>
+      </c>
+      <c r="I34" s="9">
+        <v>0</v>
+      </c>
+      <c r="J34" s="9"/>
+      <c r="K34" s="9">
+        <v>8.9789999999999992</v>
+      </c>
+      <c r="L34" s="9">
+        <v>0</v>
+      </c>
+      <c r="M34" s="9"/>
+      <c r="N34" s="9"/>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A35" s="15"/>
+      <c r="B35" s="11">
+        <v>33483</v>
+      </c>
+      <c r="C35" s="9"/>
+      <c r="D35" s="9">
+        <v>91.39500000000001</v>
+      </c>
+      <c r="E35" s="9">
+        <v>26.811500000000002</v>
+      </c>
+      <c r="F35" s="9">
+        <v>87.9</v>
+      </c>
+      <c r="G35" s="9">
+        <v>1.415</v>
+      </c>
+      <c r="H35" s="9">
+        <v>47.5</v>
+      </c>
+      <c r="I35" s="9">
+        <v>0</v>
+      </c>
+      <c r="J35" s="9"/>
+      <c r="K35" s="9">
+        <v>60.523499999999999</v>
+      </c>
+      <c r="L35" s="9">
+        <v>0.58850000000000002</v>
+      </c>
+      <c r="M35" s="9"/>
+      <c r="N35" s="9"/>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A36" s="15"/>
+      <c r="B36" s="11">
+        <v>33504</v>
+      </c>
+      <c r="C36" s="9"/>
+      <c r="D36" s="9">
+        <v>88.582999999999998</v>
+      </c>
+      <c r="E36" s="9">
+        <v>169.19150000000002</v>
+      </c>
+      <c r="F36" s="9">
+        <v>312.45</v>
+      </c>
+      <c r="G36" s="9">
+        <v>4.0049999999999999</v>
+      </c>
+      <c r="H36" s="9">
+        <v>64.5</v>
+      </c>
+      <c r="I36" s="9">
+        <v>0.17699999999999999</v>
+      </c>
+      <c r="J36" s="9">
+        <v>0</v>
+      </c>
+      <c r="K36" s="9">
+        <v>137.321</v>
+      </c>
+      <c r="L36" s="9">
+        <v>5.9450000000000003</v>
+      </c>
+      <c r="M36" s="9"/>
+      <c r="N36" s="9"/>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A37" s="15"/>
+      <c r="B37" s="11">
+        <v>33512</v>
+      </c>
+      <c r="C37" s="9"/>
+      <c r="D37" s="9">
+        <v>92.801000000000002</v>
+      </c>
+      <c r="E37" s="9">
+        <v>268.75400000000002</v>
+      </c>
+      <c r="F37" s="9">
+        <v>456.8</v>
+      </c>
+      <c r="G37" s="9">
+        <v>3.96</v>
+      </c>
+      <c r="H37" s="9">
+        <v>72</v>
+      </c>
+      <c r="I37" s="9">
+        <v>32.164500000000004</v>
+      </c>
+      <c r="J37" s="9">
+        <v>0</v>
+      </c>
+      <c r="K37" s="9">
+        <v>137.80350000000001</v>
+      </c>
+      <c r="L37" s="9">
+        <v>13.5395</v>
+      </c>
+      <c r="M37" s="9"/>
+      <c r="N37" s="9"/>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A38" s="15"/>
+      <c r="B38" s="11">
+        <v>33513</v>
+      </c>
+      <c r="C38" s="9">
+        <v>7</v>
+      </c>
+      <c r="D38" s="9"/>
+      <c r="E38" s="9"/>
+      <c r="F38" s="9"/>
+      <c r="G38" s="9"/>
+      <c r="H38" s="9"/>
+      <c r="I38" s="9"/>
+      <c r="J38" s="9"/>
+      <c r="K38" s="9"/>
+      <c r="L38" s="9"/>
+      <c r="M38" s="9"/>
+      <c r="N38" s="9"/>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A39" s="15"/>
+      <c r="B39" s="11">
+        <v>33518</v>
+      </c>
+      <c r="C39" s="9"/>
+      <c r="D39" s="9">
+        <v>89.989000000000004</v>
+      </c>
+      <c r="E39" s="9">
+        <v>357.08850000000001</v>
+      </c>
+      <c r="F39" s="9">
+        <v>623.90000000000009</v>
+      </c>
+      <c r="G39" s="9">
+        <v>3.45</v>
+      </c>
+      <c r="H39" s="9">
+        <v>72</v>
+      </c>
+      <c r="I39" s="9">
+        <v>119.4555</v>
+      </c>
+      <c r="J39" s="9">
+        <v>352.92449999999997</v>
+      </c>
+      <c r="K39" s="9">
+        <v>125.92699999999999</v>
+      </c>
+      <c r="L39" s="9">
+        <v>23.974</v>
+      </c>
+      <c r="M39" s="9"/>
+      <c r="N39" s="9"/>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A40" s="15"/>
+      <c r="B40" s="11">
+        <v>33525</v>
+      </c>
+      <c r="C40" s="9"/>
+      <c r="D40" s="9">
+        <v>95.613</v>
+      </c>
+      <c r="E40" s="9">
+        <v>369.73849999999999</v>
+      </c>
+      <c r="F40" s="9">
+        <v>694.09999999999991</v>
+      </c>
+      <c r="G40" s="9">
+        <v>2.5949999999999998</v>
+      </c>
+      <c r="H40" s="9">
+        <v>76.5</v>
+      </c>
+      <c r="I40" s="9">
+        <v>167.85250000000002</v>
+      </c>
+      <c r="J40" s="9">
+        <v>385.2645</v>
+      </c>
+      <c r="K40" s="9">
+        <v>106.3685</v>
+      </c>
+      <c r="L40" s="9">
+        <v>30.823</v>
+      </c>
+      <c r="M40" s="9"/>
+      <c r="N40" s="9"/>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A41" s="15"/>
+      <c r="B41" s="11">
+        <v>33532</v>
+      </c>
+      <c r="C41" s="9"/>
+      <c r="D41" s="9">
+        <v>94.206999999999994</v>
+      </c>
+      <c r="E41" s="9">
+        <v>406.22550000000001</v>
+      </c>
+      <c r="F41" s="9">
+        <v>862.40000000000009</v>
+      </c>
+      <c r="G41" s="9">
+        <v>2.67</v>
+      </c>
+      <c r="H41" s="9">
+        <v>74</v>
+      </c>
+      <c r="I41" s="9">
+        <v>308.3175</v>
+      </c>
+      <c r="J41" s="9">
+        <v>469.62900000000002</v>
+      </c>
+      <c r="K41" s="9">
+        <v>97.634500000000003</v>
+      </c>
+      <c r="L41" s="9">
+        <v>38.8825</v>
+      </c>
+      <c r="M41" s="9"/>
+      <c r="N41" s="9"/>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A42" s="15"/>
+      <c r="B42" s="11">
+        <v>33539</v>
+      </c>
+      <c r="C42" s="9"/>
+      <c r="D42" s="9">
+        <v>89.989000000000004</v>
+      </c>
+      <c r="E42" s="9">
+        <v>404.30599999999998</v>
+      </c>
+      <c r="F42" s="9">
+        <v>945.85</v>
+      </c>
+      <c r="G42" s="9">
+        <v>1.2850000000000001</v>
+      </c>
+      <c r="H42" s="9">
+        <v>77.5</v>
+      </c>
+      <c r="I42" s="9">
+        <v>397.786</v>
+      </c>
+      <c r="J42" s="9">
+        <v>427.44650000000001</v>
+      </c>
+      <c r="K42" s="9">
+        <v>60.980000000000004</v>
+      </c>
+      <c r="L42" s="9">
+        <v>72.403000000000006</v>
+      </c>
+      <c r="M42" s="9"/>
+      <c r="N42" s="9"/>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A43" s="15"/>
+      <c r="B43" s="11">
+        <v>33546</v>
+      </c>
+      <c r="C43" s="9"/>
+      <c r="D43" s="9">
+        <v>97.019000000000005</v>
+      </c>
+      <c r="E43" s="9"/>
+      <c r="F43" s="9">
+        <v>1042</v>
+      </c>
+      <c r="G43" s="9">
+        <v>0.62</v>
+      </c>
+      <c r="H43" s="9">
+        <v>73.5</v>
+      </c>
+      <c r="I43" s="9">
+        <v>509.1345</v>
+      </c>
+      <c r="J43" s="9">
+        <v>503.37450000000001</v>
+      </c>
+      <c r="K43" s="9">
+        <v>23.896000000000001</v>
+      </c>
+      <c r="L43" s="9">
+        <v>95.6935</v>
+      </c>
+      <c r="M43" s="9"/>
+      <c r="N43" s="9"/>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A44" s="15"/>
+      <c r="B44" s="11">
+        <v>33553</v>
+      </c>
+      <c r="C44" s="9"/>
+      <c r="D44" s="9">
+        <v>94.206999999999994</v>
+      </c>
+      <c r="E44" s="9"/>
+      <c r="F44" s="9">
+        <v>934.55</v>
+      </c>
+      <c r="G44" s="9">
+        <v>0.04</v>
+      </c>
+      <c r="H44" s="9"/>
+      <c r="I44" s="9">
+        <v>467.82950000000005</v>
+      </c>
+      <c r="J44" s="9">
+        <v>466.81650000000002</v>
+      </c>
+      <c r="K44" s="9">
+        <v>1.0665</v>
+      </c>
+      <c r="L44" s="9">
+        <v>96.275499999999994</v>
+      </c>
+      <c r="M44" s="9"/>
+      <c r="N44" s="9"/>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A45" s="16"/>
+      <c r="B45" s="11">
+        <v>33560</v>
+      </c>
+      <c r="C45" s="9">
+        <v>10</v>
+      </c>
+      <c r="D45" s="9">
+        <v>97.019000000000005</v>
+      </c>
+      <c r="E45" s="9"/>
+      <c r="F45" s="9">
+        <v>1049.5</v>
+      </c>
+      <c r="G45" s="9"/>
+      <c r="H45" s="9"/>
+      <c r="I45" s="9"/>
+      <c r="J45" s="9">
+        <v>400.35699999999997</v>
+      </c>
+      <c r="K45" s="9"/>
+      <c r="L45" s="9"/>
+      <c r="M45" s="9">
+        <v>431.13049999999998</v>
+      </c>
+      <c r="N45" s="9">
+        <v>4.2832699999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix date format problem
</commit_message>
<xml_diff>
--- a/Prototypes/Barley/Observed.xlsx
+++ b/Prototypes/Barley/Observed.xlsx
@@ -17465,7 +17465,7 @@
         <v>540.0141553</v>
       </c>
     </row>
-    <row r="241" spans="1:60">
+    <row r="241" spans="1:52">
       <c r="A241" s="1" t="s">
         <v>98</v>
       </c>
@@ -17500,7 +17500,7 @@
         <v>661.6644492</v>
       </c>
     </row>
-    <row r="242" spans="1:60">
+    <row r="242" spans="1:52">
       <c r="A242" s="1" t="s">
         <v>98</v>
       </c>
@@ -17562,7 +17562,7 @@
         <v>0.193333333333333</v>
       </c>
     </row>
-    <row r="243" spans="1:60">
+    <row r="243" spans="1:52">
       <c r="A243" s="1" t="s">
         <v>98</v>
       </c>
@@ -17597,7 +17597,7 @@
         <v>542.7291579</v>
       </c>
     </row>
-    <row r="244" spans="1:60">
+    <row r="244" spans="1:52">
       <c r="A244" s="1" t="s">
         <v>99</v>
       </c>
@@ -17635,7 +17635,7 @@
         <v>0.35046</v>
       </c>
     </row>
-    <row r="245" spans="1:60">
+    <row r="245" spans="1:52">
       <c r="A245" s="1" t="s">
         <v>99</v>
       </c>
@@ -17673,7 +17673,7 @@
         <v>0.35333</v>
       </c>
     </row>
-    <row r="246" spans="1:60">
+    <row r="246" spans="1:52">
       <c r="A246" s="1" t="s">
         <v>99</v>
       </c>
@@ -17684,24 +17684,45 @@
         <v>292.0833333</v>
       </c>
     </row>
-    <row r="247" spans="1:60">
+    <row r="247" spans="1:52">
       <c r="A247" s="1" t="s">
         <v>99</v>
       </c>
       <c r="B247" s="2">
-        <v>40827</v>
+        <v>40857</v>
       </c>
       <c r="G247">
         <v>705.9035765</v>
       </c>
-      <c r="BG247">
-        <v>7.45</v>
-      </c>
-      <c r="BH247">
-        <v>5.6</v>
-      </c>
-    </row>
-    <row r="248" spans="1:60">
+      <c r="AH247">
+        <v>481.3</v>
+      </c>
+      <c r="AK247">
+        <v>0.246</v>
+      </c>
+      <c r="AN247">
+        <v>0.257333333333333</v>
+      </c>
+      <c r="AP247">
+        <v>0.274166666666667</v>
+      </c>
+      <c r="AR247">
+        <v>0.285833333333333</v>
+      </c>
+      <c r="AT247">
+        <v>0.316833333333333</v>
+      </c>
+      <c r="AV247">
+        <v>0.337833333333333</v>
+      </c>
+      <c r="AX247">
+        <v>0.343333333333333</v>
+      </c>
+      <c r="AZ247">
+        <v>0.345166666666667</v>
+      </c>
+    </row>
+    <row r="248" spans="1:52">
       <c r="A248" s="1" t="s">
         <v>99</v>
       </c>
@@ -17739,7 +17760,7 @@
         <v>0.3445</v>
       </c>
     </row>
-    <row r="249" spans="1:60">
+    <row r="249" spans="1:52">
       <c r="A249" s="1" t="s">
         <v>99</v>
       </c>
@@ -17783,7 +17804,7 @@
         <v>0.345833333333333</v>
       </c>
     </row>
-    <row r="250" spans="1:60">
+    <row r="250" spans="1:52">
       <c r="A250" s="1" t="s">
         <v>99</v>
       </c>
@@ -17797,7 +17818,7 @@
         <v>1236.263333</v>
       </c>
     </row>
-    <row r="251" spans="1:60">
+    <row r="251" spans="1:52">
       <c r="A251" s="1" t="s">
         <v>100</v>
       </c>
@@ -17835,7 +17856,7 @@
         <v>0.326133333333333</v>
       </c>
     </row>
-    <row r="252" spans="1:60">
+    <row r="252" spans="1:52">
       <c r="A252" s="1" t="s">
         <v>100</v>
       </c>
@@ -17873,7 +17894,7 @@
         <v>0.333513333333333</v>
       </c>
     </row>
-    <row r="253" spans="1:60">
+    <row r="253" spans="1:52">
       <c r="A253" s="1" t="s">
         <v>100</v>
       </c>
@@ -17884,24 +17905,45 @@
         <v>335.75</v>
       </c>
     </row>
-    <row r="254" spans="1:60">
+    <row r="254" spans="1:52">
       <c r="A254" s="1" t="s">
         <v>100</v>
       </c>
       <c r="B254" s="2">
-        <v>40827</v>
+        <v>40857</v>
       </c>
       <c r="G254">
         <v>669.6128093</v>
       </c>
-      <c r="BG254">
-        <v>6.9</v>
-      </c>
-      <c r="BH254">
-        <v>5.6</v>
-      </c>
-    </row>
-    <row r="255" spans="1:60">
+      <c r="AH254">
+        <v>484.866666666667</v>
+      </c>
+      <c r="AK254">
+        <v>0.27</v>
+      </c>
+      <c r="AN254">
+        <v>0.256666666666667</v>
+      </c>
+      <c r="AP254">
+        <v>0.273166666666667</v>
+      </c>
+      <c r="AR254">
+        <v>0.289333333333333</v>
+      </c>
+      <c r="AT254">
+        <v>0.316333333333333</v>
+      </c>
+      <c r="AV254">
+        <v>0.339</v>
+      </c>
+      <c r="AX254">
+        <v>0.3395</v>
+      </c>
+      <c r="AZ254">
+        <v>0.340333333333333</v>
+      </c>
+    </row>
+    <row r="255" spans="1:52">
       <c r="A255" s="1" t="s">
         <v>100</v>
       </c>
@@ -17939,7 +17981,7 @@
         <v>0.337</v>
       </c>
     </row>
-    <row r="256" spans="1:60">
+    <row r="256" spans="1:52">
       <c r="A256" s="1" t="s">
         <v>100</v>
       </c>
@@ -17983,7 +18025,7 @@
         <v>0.3405</v>
       </c>
     </row>
-    <row r="257" spans="1:60">
+    <row r="257" spans="1:52">
       <c r="A257" s="1" t="s">
         <v>100</v>
       </c>
@@ -17997,7 +18039,7 @@
         <v>1228.483333</v>
       </c>
     </row>
-    <row r="258" spans="1:60">
+    <row r="258" spans="1:52">
       <c r="A258" s="1" t="s">
         <v>101</v>
       </c>
@@ -18035,7 +18077,7 @@
         <v>0.31848</v>
       </c>
     </row>
-    <row r="259" spans="1:60">
+    <row r="259" spans="1:52">
       <c r="A259" s="1" t="s">
         <v>101</v>
       </c>
@@ -18073,7 +18115,7 @@
         <v>0.319573333333333</v>
       </c>
     </row>
-    <row r="260" spans="1:60">
+    <row r="260" spans="1:52">
       <c r="A260" s="1" t="s">
         <v>101</v>
       </c>
@@ -18084,24 +18126,45 @@
         <v>341.5833333</v>
       </c>
     </row>
-    <row r="261" spans="1:60">
+    <row r="261" spans="1:52">
       <c r="A261" s="1" t="s">
         <v>101</v>
       </c>
       <c r="B261" s="2">
-        <v>40827</v>
+        <v>40857</v>
       </c>
       <c r="G261">
         <v>796.2793878</v>
       </c>
-      <c r="BG261">
-        <v>7</v>
-      </c>
-      <c r="BH261">
-        <v>5.7</v>
-      </c>
-    </row>
-    <row r="262" spans="1:60">
+      <c r="AH261">
+        <v>456.966666666667</v>
+      </c>
+      <c r="AK261">
+        <v>0.2365</v>
+      </c>
+      <c r="AN261">
+        <v>0.243166666666667</v>
+      </c>
+      <c r="AP261">
+        <v>0.265833333333333</v>
+      </c>
+      <c r="AR261">
+        <v>0.271166666666667</v>
+      </c>
+      <c r="AT261">
+        <v>0.301166666666667</v>
+      </c>
+      <c r="AV261">
+        <v>0.330833333333333</v>
+      </c>
+      <c r="AX261">
+        <v>0.327</v>
+      </c>
+      <c r="AZ261">
+        <v>0.309166666666667</v>
+      </c>
+    </row>
+    <row r="262" spans="1:52">
       <c r="A262" s="1" t="s">
         <v>101</v>
       </c>
@@ -18139,7 +18202,7 @@
         <v>0.306833333333333</v>
       </c>
     </row>
-    <row r="263" spans="1:60">
+    <row r="263" spans="1:52">
       <c r="A263" s="1" t="s">
         <v>101</v>
       </c>
@@ -18183,7 +18246,7 @@
         <v>0.309833333333333</v>
       </c>
     </row>
-    <row r="264" spans="1:60">
+    <row r="264" spans="1:52">
       <c r="A264" s="1" t="s">
         <v>101</v>
       </c>
@@ -18197,7 +18260,7 @@
         <v>1112.343333</v>
       </c>
     </row>
-    <row r="265" spans="1:60">
+    <row r="265" spans="1:52">
       <c r="A265" s="1" t="s">
         <v>102</v>
       </c>
@@ -18235,7 +18298,7 @@
         <v>0.329686666666667</v>
       </c>
     </row>
-    <row r="266" spans="1:60">
+    <row r="266" spans="1:52">
       <c r="A266" s="1" t="s">
         <v>102</v>
       </c>
@@ -18246,24 +18309,45 @@
         <v>41.60833333</v>
       </c>
     </row>
-    <row r="267" spans="1:60">
+    <row r="267" spans="1:52">
       <c r="A267" s="1" t="s">
         <v>102</v>
       </c>
       <c r="B267" s="2">
-        <v>40827</v>
+        <v>40857</v>
       </c>
       <c r="G267">
         <v>156.6666667</v>
       </c>
-      <c r="BG267">
-        <v>3</v>
-      </c>
-      <c r="BH267">
-        <v>1.9</v>
-      </c>
-    </row>
-    <row r="268" spans="1:60">
+      <c r="AH267">
+        <v>506.433333333333</v>
+      </c>
+      <c r="AK267">
+        <v>0.297166666666667</v>
+      </c>
+      <c r="AN267">
+        <v>0.2875</v>
+      </c>
+      <c r="AP267">
+        <v>0.295666666666667</v>
+      </c>
+      <c r="AR267">
+        <v>0.2995</v>
+      </c>
+      <c r="AT267">
+        <v>0.321333333333333</v>
+      </c>
+      <c r="AV267">
+        <v>0.342333333333333</v>
+      </c>
+      <c r="AX267">
+        <v>0.348</v>
+      </c>
+      <c r="AZ267">
+        <v>0.340666666666667</v>
+      </c>
+    </row>
+    <row r="268" spans="1:52">
       <c r="A268" s="1" t="s">
         <v>102</v>
       </c>
@@ -18301,34 +18385,88 @@
         <v>0.3335</v>
       </c>
     </row>
-    <row r="269" spans="1:60">
+    <row r="269" spans="1:52">
       <c r="A269" s="1" t="s">
         <v>102</v>
       </c>
       <c r="B269" s="2">
-        <v>40767</v>
+        <v>40885</v>
       </c>
       <c r="G269">
         <v>1014.742537</v>
       </c>
-    </row>
-    <row r="270" spans="1:60">
+      <c r="AH269">
+        <v>457.566666666667</v>
+      </c>
+      <c r="AK269">
+        <v>0.280666666666667</v>
+      </c>
+      <c r="AN269">
+        <v>0.246166666666667</v>
+      </c>
+      <c r="AP269">
+        <v>0.240333333333333</v>
+      </c>
+      <c r="AR269">
+        <v>0.2445</v>
+      </c>
+      <c r="AT269">
+        <v>0.289166666666667</v>
+      </c>
+      <c r="AV269">
+        <v>0.316166666666667</v>
+      </c>
+      <c r="AX269">
+        <v>0.3395</v>
+      </c>
+      <c r="AZ269">
+        <v>0.331333333333333</v>
+      </c>
+    </row>
+    <row r="270" spans="1:52">
       <c r="A270" s="1" t="s">
         <v>102</v>
       </c>
       <c r="B270" s="2">
-        <v>41030</v>
+        <v>40913</v>
       </c>
       <c r="G270">
         <v>1872.216922</v>
       </c>
-    </row>
-    <row r="271" spans="1:60">
+      <c r="AH270">
+        <v>442.1</v>
+      </c>
+      <c r="AK270">
+        <v>0.285666666666667</v>
+      </c>
+      <c r="AN270">
+        <v>0.252833333333333</v>
+      </c>
+      <c r="AP270">
+        <v>0.226833333333333</v>
+      </c>
+      <c r="AR270">
+        <v>0.2245</v>
+      </c>
+      <c r="AT270">
+        <v>0.2685</v>
+      </c>
+      <c r="AV270">
+        <v>0.290166666666667</v>
+      </c>
+      <c r="AX270">
+        <v>0.331666666666667</v>
+      </c>
+      <c r="AZ270">
+        <v>0.330333333333333</v>
+      </c>
+    </row>
+    <row r="271" spans="1:52">
       <c r="A271" s="1" t="s">
         <v>102</v>
       </c>
       <c r="B271" s="2">
-        <v>41154</v>
+        <v>40948</v>
       </c>
       <c r="G271">
         <v>1746.218918</v>
@@ -18336,8 +18474,35 @@
       <c r="N271">
         <v>1176.403333</v>
       </c>
-    </row>
-    <row r="272" spans="1:60">
+      <c r="AH271">
+        <v>383.433333333333</v>
+      </c>
+      <c r="AK271">
+        <v>0.1845</v>
+      </c>
+      <c r="AN271">
+        <v>0.215166666666667</v>
+      </c>
+      <c r="AP271">
+        <v>0.207833333333333</v>
+      </c>
+      <c r="AR271">
+        <v>0.201666666666667</v>
+      </c>
+      <c r="AT271">
+        <v>0.233666666666667</v>
+      </c>
+      <c r="AV271">
+        <v>0.238833333333333</v>
+      </c>
+      <c r="AX271">
+        <v>0.319333333333333</v>
+      </c>
+      <c r="AZ271">
+        <v>0.316166666666667</v>
+      </c>
+    </row>
+    <row r="272" spans="1:52">
       <c r="A272" s="1" t="s">
         <v>103</v>
       </c>
@@ -18375,7 +18540,7 @@
         <v>0.33734</v>
       </c>
     </row>
-    <row r="273" spans="1:60">
+    <row r="273" spans="1:52">
       <c r="A273" s="1" t="s">
         <v>103</v>
       </c>
@@ -18386,24 +18551,45 @@
         <v>48.46666667</v>
       </c>
     </row>
-    <row r="274" spans="1:60">
+    <row r="274" spans="1:52">
       <c r="A274" s="1" t="s">
         <v>103</v>
       </c>
       <c r="B274" s="2">
-        <v>40827</v>
+        <v>40857</v>
       </c>
       <c r="G274">
         <v>188.75</v>
       </c>
-      <c r="BG274">
-        <v>3</v>
-      </c>
-      <c r="BH274">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="275" spans="1:60">
+      <c r="AH274">
+        <v>497.1</v>
+      </c>
+      <c r="AK274">
+        <v>0.295</v>
+      </c>
+      <c r="AN274">
+        <v>0.276</v>
+      </c>
+      <c r="AP274">
+        <v>0.2895</v>
+      </c>
+      <c r="AR274">
+        <v>0.304166666666667</v>
+      </c>
+      <c r="AT274">
+        <v>0.3135</v>
+      </c>
+      <c r="AV274">
+        <v>0.3385</v>
+      </c>
+      <c r="AX274">
+        <v>0.337166666666667</v>
+      </c>
+      <c r="AZ274">
+        <v>0.331666666666667</v>
+      </c>
+    </row>
+    <row r="275" spans="1:52">
       <c r="A275" s="1" t="s">
         <v>103</v>
       </c>
@@ -18441,34 +18627,88 @@
         <v>0.328666666666667</v>
       </c>
     </row>
-    <row r="276" spans="1:60">
+    <row r="276" spans="1:52">
       <c r="A276" s="1" t="s">
         <v>103</v>
       </c>
       <c r="B276" s="2">
-        <v>40767</v>
+        <v>40885</v>
       </c>
       <c r="G276">
         <v>1023.785242</v>
       </c>
-    </row>
-    <row r="277" spans="1:60">
+      <c r="AH276">
+        <v>459.5</v>
+      </c>
+      <c r="AK276">
+        <v>0.295833333333333</v>
+      </c>
+      <c r="AN276">
+        <v>0.248166666666667</v>
+      </c>
+      <c r="AP276">
+        <v>0.237833333333333</v>
+      </c>
+      <c r="AR276">
+        <v>0.260666666666667</v>
+      </c>
+      <c r="AT276">
+        <v>0.2785</v>
+      </c>
+      <c r="AV276">
+        <v>0.316166666666667</v>
+      </c>
+      <c r="AX276">
+        <v>0.331833333333333</v>
+      </c>
+      <c r="AZ276">
+        <v>0.3285</v>
+      </c>
+    </row>
+    <row r="277" spans="1:52">
       <c r="A277" s="1" t="s">
         <v>103</v>
       </c>
       <c r="B277" s="2">
-        <v>41030</v>
+        <v>40913</v>
       </c>
       <c r="G277">
         <v>1810.57359</v>
       </c>
-    </row>
-    <row r="278" spans="1:60">
+      <c r="AH277">
+        <v>444.033333333333</v>
+      </c>
+      <c r="AK277">
+        <v>0.295333333333333</v>
+      </c>
+      <c r="AN277">
+        <v>0.254</v>
+      </c>
+      <c r="AP277">
+        <v>0.2345</v>
+      </c>
+      <c r="AR277">
+        <v>0.2415</v>
+      </c>
+      <c r="AT277">
+        <v>0.25</v>
+      </c>
+      <c r="AV277">
+        <v>0.291333333333333</v>
+      </c>
+      <c r="AX277">
+        <v>0.3265</v>
+      </c>
+      <c r="AZ277">
+        <v>0.327</v>
+      </c>
+    </row>
+    <row r="278" spans="1:52">
       <c r="A278" s="1" t="s">
         <v>103</v>
       </c>
       <c r="B278" s="2">
-        <v>41154</v>
+        <v>40948</v>
       </c>
       <c r="G278">
         <v>1930.599592</v>
@@ -18476,8 +18716,35 @@
       <c r="N278">
         <v>1236.823333</v>
       </c>
-    </row>
-    <row r="279" spans="1:60">
+      <c r="AH278">
+        <v>385.533333333333</v>
+      </c>
+      <c r="AK278">
+        <v>0.178333333333333</v>
+      </c>
+      <c r="AN278">
+        <v>0.222</v>
+      </c>
+      <c r="AP278">
+        <v>0.221666666666667</v>
+      </c>
+      <c r="AR278">
+        <v>0.206166666666667</v>
+      </c>
+      <c r="AT278">
+        <v>0.2085</v>
+      </c>
+      <c r="AV278">
+        <v>0.250666666666667</v>
+      </c>
+      <c r="AX278">
+        <v>0.313666666666667</v>
+      </c>
+      <c r="AZ278">
+        <v>0.326666666666667</v>
+      </c>
+    </row>
+    <row r="279" spans="1:52">
       <c r="A279" s="1" t="s">
         <v>104</v>
       </c>
@@ -18515,7 +18782,7 @@
         <v>0.319846666666667</v>
       </c>
     </row>
-    <row r="280" spans="1:60">
+    <row r="280" spans="1:52">
       <c r="A280" s="1" t="s">
         <v>104</v>
       </c>
@@ -18526,24 +18793,45 @@
         <v>59.54166667</v>
       </c>
     </row>
-    <row r="281" spans="1:60">
+    <row r="281" spans="1:52">
       <c r="A281" s="1" t="s">
         <v>104</v>
       </c>
       <c r="B281" s="2">
-        <v>40827</v>
+        <v>40857</v>
       </c>
       <c r="G281">
         <v>209.8333333</v>
       </c>
-      <c r="BG281">
-        <v>3</v>
-      </c>
-      <c r="BH281">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="282" spans="1:60">
+      <c r="AH281">
+        <v>492.433333333333</v>
+      </c>
+      <c r="AK281">
+        <v>0.308333333333333</v>
+      </c>
+      <c r="AN281">
+        <v>0.270333333333333</v>
+      </c>
+      <c r="AP281">
+        <v>0.285</v>
+      </c>
+      <c r="AR281">
+        <v>0.292166666666667</v>
+      </c>
+      <c r="AT281">
+        <v>0.3155</v>
+      </c>
+      <c r="AV281">
+        <v>0.337833333333333</v>
+      </c>
+      <c r="AX281">
+        <v>0.326333333333333</v>
+      </c>
+      <c r="AZ281">
+        <v>0.326666666666667</v>
+      </c>
+    </row>
+    <row r="282" spans="1:52">
       <c r="A282" s="1" t="s">
         <v>104</v>
       </c>
@@ -18581,34 +18869,88 @@
         <v>0.321833333333333</v>
       </c>
     </row>
-    <row r="283" spans="1:60">
+    <row r="283" spans="1:52">
       <c r="A283" s="1" t="s">
         <v>104</v>
       </c>
       <c r="B283" s="2">
-        <v>40767</v>
+        <v>40885</v>
       </c>
       <c r="G283">
         <v>981.1406696</v>
       </c>
-    </row>
-    <row r="284" spans="1:60">
+      <c r="AH283">
+        <v>453.566666666667</v>
+      </c>
+      <c r="AK283">
+        <v>0.295333333333333</v>
+      </c>
+      <c r="AN283">
+        <v>0.258666666666667</v>
+      </c>
+      <c r="AP283">
+        <v>0.246166666666667</v>
+      </c>
+      <c r="AR283">
+        <v>0.239333333333333</v>
+      </c>
+      <c r="AT283">
+        <v>0.267166666666667</v>
+      </c>
+      <c r="AV283">
+        <v>0.318166666666667</v>
+      </c>
+      <c r="AX283">
+        <v>0.318833333333333</v>
+      </c>
+      <c r="AZ283">
+        <v>0.324166666666667</v>
+      </c>
+    </row>
+    <row r="284" spans="1:52">
       <c r="A284" s="1" t="s">
         <v>104</v>
       </c>
       <c r="B284" s="2">
-        <v>41030</v>
+        <v>40913</v>
       </c>
       <c r="G284">
         <v>1791.889429</v>
       </c>
-    </row>
-    <row r="285" spans="1:60">
+      <c r="AH284">
+        <v>434.466666666667</v>
+      </c>
+      <c r="AK284">
+        <v>0.2835</v>
+      </c>
+      <c r="AN284">
+        <v>0.272833333333333</v>
+      </c>
+      <c r="AP284">
+        <v>0.2445</v>
+      </c>
+      <c r="AR284">
+        <v>0.222666666666667</v>
+      </c>
+      <c r="AT284">
+        <v>0.2265</v>
+      </c>
+      <c r="AV284">
+        <v>0.295833333333333</v>
+      </c>
+      <c r="AX284">
+        <v>0.307</v>
+      </c>
+      <c r="AZ284">
+        <v>0.3195</v>
+      </c>
+    </row>
+    <row r="285" spans="1:52">
       <c r="A285" s="1" t="s">
         <v>104</v>
       </c>
       <c r="B285" s="2">
-        <v>41154</v>
+        <v>40948</v>
       </c>
       <c r="G285">
         <v>1622.906238</v>
@@ -18616,19 +18958,73 @@
       <c r="N285">
         <v>905.1933333</v>
       </c>
-    </row>
-    <row r="286" spans="1:60">
+      <c r="AH285">
+        <v>382.033333333333</v>
+      </c>
+      <c r="AK285">
+        <v>0.1685</v>
+      </c>
+      <c r="AN285">
+        <v>0.236333333333333</v>
+      </c>
+      <c r="AP285">
+        <v>0.230833333333333</v>
+      </c>
+      <c r="AR285">
+        <v>0.196166666666667</v>
+      </c>
+      <c r="AT285">
+        <v>0.197666666666667</v>
+      </c>
+      <c r="AV285">
+        <v>0.266833333333333</v>
+      </c>
+      <c r="AX285">
+        <v>0.299166666666667</v>
+      </c>
+      <c r="AZ285">
+        <v>0.314666666666667</v>
+      </c>
+    </row>
+    <row r="286" spans="1:52">
       <c r="A286" s="1" t="s">
         <v>105</v>
       </c>
       <c r="B286" s="2">
-        <v>40767</v>
+        <v>40885</v>
       </c>
       <c r="G286">
         <v>27.5</v>
       </c>
-    </row>
-    <row r="287" spans="1:60">
+      <c r="AH286">
+        <v>505.966666666667</v>
+      </c>
+      <c r="AK286">
+        <v>0.331166666666667</v>
+      </c>
+      <c r="AN286">
+        <v>0.323</v>
+      </c>
+      <c r="AP286">
+        <v>0.309166666666667</v>
+      </c>
+      <c r="AR286">
+        <v>0.309666666666667</v>
+      </c>
+      <c r="AT286">
+        <v>0.302</v>
+      </c>
+      <c r="AV286">
+        <v>0.322</v>
+      </c>
+      <c r="AX286">
+        <v>0.317666666666667</v>
+      </c>
+      <c r="AZ286">
+        <v>0.315166666666667</v>
+      </c>
+    </row>
+    <row r="287" spans="1:52">
       <c r="A287" s="1" t="s">
         <v>105</v>
       </c>
@@ -18672,15 +19068,42 @@
         <v>0.315833333333333</v>
       </c>
     </row>
-    <row r="288" spans="1:60">
+    <row r="288" spans="1:52">
       <c r="A288" s="1" t="s">
         <v>105</v>
       </c>
       <c r="B288" s="2">
-        <v>41030</v>
+        <v>40913</v>
       </c>
       <c r="G288">
         <v>597.7025821</v>
+      </c>
+      <c r="AH288">
+        <v>469.533333333333</v>
+      </c>
+      <c r="AK288">
+        <v>0.3015</v>
+      </c>
+      <c r="AN288">
+        <v>0.263333333333333</v>
+      </c>
+      <c r="AP288">
+        <v>0.279666666666667</v>
+      </c>
+      <c r="AR288">
+        <v>0.281</v>
+      </c>
+      <c r="AT288">
+        <v>0.277666666666667</v>
+      </c>
+      <c r="AV288">
+        <v>0.312</v>
+      </c>
+      <c r="AX288">
+        <v>0.314</v>
+      </c>
+      <c r="AZ288">
+        <v>0.3185</v>
       </c>
     </row>
     <row r="289" spans="1:52">
@@ -18805,10 +19228,37 @@
         <v>106</v>
       </c>
       <c r="B292" s="2">
-        <v>40767</v>
+        <v>40885</v>
       </c>
       <c r="G292">
         <v>26.75</v>
+      </c>
+      <c r="AH292">
+        <v>501.966666666667</v>
+      </c>
+      <c r="AK292">
+        <v>0.314166666666667</v>
+      </c>
+      <c r="AN292">
+        <v>0.32</v>
+      </c>
+      <c r="AP292">
+        <v>0.306</v>
+      </c>
+      <c r="AR292">
+        <v>0.287666666666667</v>
+      </c>
+      <c r="AT292">
+        <v>0.3055</v>
+      </c>
+      <c r="AV292">
+        <v>0.3205</v>
+      </c>
+      <c r="AX292">
+        <v>0.335333333333333</v>
+      </c>
+      <c r="AZ292">
+        <v>0.320666666666667</v>
       </c>
     </row>
     <row r="293" spans="1:52">
@@ -18860,10 +19310,37 @@
         <v>106</v>
       </c>
       <c r="B294" s="2">
-        <v>41030</v>
+        <v>40913</v>
       </c>
       <c r="G294">
         <v>597.1387123</v>
+      </c>
+      <c r="AH294">
+        <v>464.033333333333</v>
+      </c>
+      <c r="AK294">
+        <v>0.2855</v>
+      </c>
+      <c r="AN294">
+        <v>0.2675</v>
+      </c>
+      <c r="AP294">
+        <v>0.2725</v>
+      </c>
+      <c r="AR294">
+        <v>0.251833333333333</v>
+      </c>
+      <c r="AT294">
+        <v>0.280333333333333</v>
+      </c>
+      <c r="AV294">
+        <v>0.309666666666667</v>
+      </c>
+      <c r="AX294">
+        <v>0.331</v>
+      </c>
+      <c r="AZ294">
+        <v>0.321833333333333</v>
       </c>
     </row>
     <row r="295" spans="1:52">
@@ -18988,10 +19465,37 @@
         <v>107</v>
       </c>
       <c r="B298" s="2">
-        <v>40767</v>
+        <v>40885</v>
       </c>
       <c r="G298">
         <v>27.66666667</v>
+      </c>
+      <c r="AH298">
+        <v>500.533333333333</v>
+      </c>
+      <c r="AK298">
+        <v>0.314666666666667</v>
+      </c>
+      <c r="AN298">
+        <v>0.325833333333333</v>
+      </c>
+      <c r="AP298">
+        <v>0.306333333333333</v>
+      </c>
+      <c r="AR298">
+        <v>0.296333333333333</v>
+      </c>
+      <c r="AT298">
+        <v>0.314333333333333</v>
+      </c>
+      <c r="AV298">
+        <v>0.321666666666667</v>
+      </c>
+      <c r="AX298">
+        <v>0.3135</v>
+      </c>
+      <c r="AZ298">
+        <v>0.31</v>
       </c>
     </row>
     <row r="299" spans="1:52">
@@ -19043,10 +19547,37 @@
         <v>107</v>
       </c>
       <c r="B300" s="2">
-        <v>41030</v>
+        <v>40913</v>
       </c>
       <c r="G300">
         <v>599.8234083</v>
+      </c>
+      <c r="AH300">
+        <v>456.1</v>
+      </c>
+      <c r="AK300">
+        <v>0.276666666666667</v>
+      </c>
+      <c r="AN300">
+        <v>0.261166666666667</v>
+      </c>
+      <c r="AP300">
+        <v>0.270166666666667</v>
+      </c>
+      <c r="AR300">
+        <v>0.262333333333333</v>
+      </c>
+      <c r="AT300">
+        <v>0.283666666666667</v>
+      </c>
+      <c r="AV300">
+        <v>0.307333333333333</v>
+      </c>
+      <c r="AX300">
+        <v>0.307333333333333</v>
+      </c>
+      <c r="AZ300">
+        <v>0.311833333333333</v>
       </c>
     </row>
     <row r="301" spans="1:52">
@@ -52874,6 +53405,9 @@
       <c r="B1070" s="2">
         <v>40857</v>
       </c>
+      <c r="G1070">
+        <v>705.9035765</v>
+      </c>
       <c r="AH1070">
         <v>481.3</v>
       </c>
@@ -53218,6 +53752,9 @@
       <c r="B1083" s="2">
         <v>40857</v>
       </c>
+      <c r="G1083">
+        <v>669.6128093</v>
+      </c>
       <c r="AH1083">
         <v>484.866666666667</v>
       </c>
@@ -53562,6 +54099,9 @@
       <c r="B1096" s="2">
         <v>40857</v>
       </c>
+      <c r="G1096">
+        <v>796.2793878</v>
+      </c>
       <c r="AH1096">
         <v>456.966666666667</v>
       </c>
@@ -53849,6 +54389,9 @@
       <c r="B1109" s="2">
         <v>40857</v>
       </c>
+      <c r="G1109">
+        <v>156.6666667</v>
+      </c>
       <c r="AH1109">
         <v>506.433333333333</v>
       </c>
@@ -53922,6 +54465,9 @@
       <c r="B1111" s="2">
         <v>40885</v>
       </c>
+      <c r="G1111">
+        <v>1014.742537</v>
+      </c>
       <c r="AH1111">
         <v>457.566666666667</v>
       </c>
@@ -53971,6 +54517,9 @@
       <c r="B1113" s="2">
         <v>40913</v>
       </c>
+      <c r="G1113">
+        <v>1872.216922</v>
+      </c>
       <c r="AH1113">
         <v>442.1</v>
       </c>
@@ -54022,6 +54571,12 @@
       <c r="B1116" s="2">
         <v>40948</v>
       </c>
+      <c r="G1116">
+        <v>1746.218918</v>
+      </c>
+      <c r="N1116">
+        <v>1176.403333</v>
+      </c>
       <c r="AH1116">
         <v>383.433333333333</v>
       </c>
@@ -54160,6 +54715,9 @@
       <c r="B1122" s="2">
         <v>40857</v>
       </c>
+      <c r="G1122">
+        <v>188.75</v>
+      </c>
       <c r="AH1122">
         <v>497.1</v>
       </c>
@@ -54233,6 +54791,9 @@
       <c r="B1124" s="2">
         <v>40885</v>
       </c>
+      <c r="G1124">
+        <v>1023.785242</v>
+      </c>
       <c r="AH1124">
         <v>459.5</v>
       </c>
@@ -54282,6 +54843,9 @@
       <c r="B1126" s="2">
         <v>40913</v>
       </c>
+      <c r="G1126">
+        <v>1810.57359</v>
+      </c>
       <c r="AH1126">
         <v>444.033333333333</v>
       </c>
@@ -54333,6 +54897,12 @@
       <c r="B1129" s="2">
         <v>40948</v>
       </c>
+      <c r="G1129">
+        <v>1930.599592</v>
+      </c>
+      <c r="N1129">
+        <v>1236.823333</v>
+      </c>
       <c r="AH1129">
         <v>385.533333333333</v>
       </c>
@@ -54471,6 +55041,9 @@
       <c r="B1135" s="2">
         <v>40857</v>
       </c>
+      <c r="G1135">
+        <v>209.8333333</v>
+      </c>
       <c r="AH1135">
         <v>492.433333333333</v>
       </c>
@@ -54544,6 +55117,9 @@
       <c r="B1137" s="2">
         <v>40885</v>
       </c>
+      <c r="G1137">
+        <v>981.1406696</v>
+      </c>
       <c r="AH1137">
         <v>453.566666666667</v>
       </c>
@@ -54593,6 +55169,9 @@
       <c r="B1139" s="2">
         <v>40913</v>
       </c>
+      <c r="G1139">
+        <v>1791.889429</v>
+      </c>
       <c r="AH1139">
         <v>434.466666666667</v>
       </c>
@@ -54644,6 +55223,12 @@
       <c r="B1142" s="2">
         <v>40948</v>
       </c>
+      <c r="G1142">
+        <v>1622.906238</v>
+      </c>
+      <c r="N1142">
+        <v>905.1933333</v>
+      </c>
       <c r="AH1142">
         <v>382.033333333333</v>
       </c>
@@ -54735,6 +55320,9 @@
       <c r="B1150" s="2">
         <v>40885</v>
       </c>
+      <c r="G1150">
+        <v>27.5</v>
+      </c>
       <c r="AH1150">
         <v>505.966666666667</v>
       </c>
@@ -54814,6 +55402,9 @@
       <c r="B1152" s="2">
         <v>40913</v>
       </c>
+      <c r="G1152">
+        <v>597.7025821</v>
+      </c>
       <c r="AH1152">
         <v>469.533333333333</v>
       </c>
@@ -55022,6 +55613,9 @@
       <c r="B1163" s="2">
         <v>40885</v>
       </c>
+      <c r="G1163">
+        <v>26.75</v>
+      </c>
       <c r="AH1163">
         <v>501.966666666667</v>
       </c>
@@ -55101,6 +55695,9 @@
       <c r="B1165" s="2">
         <v>40913</v>
       </c>
+      <c r="G1165">
+        <v>597.1387123</v>
+      </c>
       <c r="AH1165">
         <v>464.033333333333</v>
       </c>
@@ -55309,6 +55906,9 @@
       <c r="B1176" s="2">
         <v>40885</v>
       </c>
+      <c r="G1176">
+        <v>27.66666667</v>
+      </c>
       <c r="AH1176">
         <v>500.533333333333</v>
       </c>
@@ -55388,6 +55988,9 @@
       <c r="B1178" s="2">
         <v>40913</v>
       </c>
+      <c r="G1178">
+        <v>599.8234083</v>
+      </c>
       <c r="AH1178">
         <v>456.1</v>
       </c>
@@ -100630,9 +101233,6 @@
       <c r="B2898" s="2">
         <v>40827</v>
       </c>
-      <c r="G2898">
-        <v>705.9035765</v>
-      </c>
       <c r="BG2898">
         <v>7.45</v>
       </c>
@@ -100743,9 +101343,6 @@
       <c r="B2905" s="2">
         <v>40827</v>
       </c>
-      <c r="G2905">
-        <v>669.6128093</v>
-      </c>
       <c r="BG2905">
         <v>6.9</v>
       </c>
@@ -100856,9 +101453,6 @@
       <c r="B2912" s="2">
         <v>40827</v>
       </c>
-      <c r="G2912">
-        <v>796.2793878</v>
-      </c>
       <c r="BG2912">
         <v>7</v>
       </c>
@@ -100901,9 +101495,6 @@
       <c r="B2915" s="2">
         <v>40827</v>
       </c>
-      <c r="G2915">
-        <v>156.6666667</v>
-      </c>
       <c r="BG2915">
         <v>3</v>
       </c>
@@ -100960,9 +101551,6 @@
       <c r="B2919" s="2">
         <v>40827</v>
       </c>
-      <c r="G2919">
-        <v>188.75</v>
-      </c>
       <c r="BG2919">
         <v>3</v>
       </c>
@@ -101018,9 +101606,6 @@
       </c>
       <c r="B2923" s="2">
         <v>40827</v>
-      </c>
-      <c r="G2923">
-        <v>209.8333333</v>
       </c>
       <c r="BG2923">
         <v>3</v>

</xml_diff>